<commit_message>
Updated KeepOps tasks in action list
</commit_message>
<xml_diff>
--- a/T946.1 - Trial 4 Committee Action List.xlsx
+++ b/T946.1 - Trial 4 Committee Action List.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21319"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="41" documentId="11_3633EDF22E86940C3D6A942DC90AB79D76948A8B" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{EDC663A7-2EB5-444D-A85E-FC0162AFA1D0}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="30" windowWidth="28515" windowHeight="13350" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="120" yWindow="36" windowWidth="28512" windowHeight="13356" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Trial Committee" sheetId="1" r:id="rId1"/>
@@ -16,7 +15,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Solution Providers'!$B$3:$I$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Trial Committee'!$B$3:$I$125</definedName>
   </definedNames>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -28,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="614" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="617" uniqueCount="240">
   <si>
     <t xml:space="preserve">     Trial 4 - Committee - Action List</t>
   </si>
@@ -861,15 +860,24 @@
   <si>
     <t>Use case - adding messages</t>
   </si>
+  <si>
+    <t>Routes can obtained via the web interface</t>
+  </si>
+  <si>
+    <t>Done, however still not fully clear if this a usecase</t>
+  </si>
+  <si>
+    <t>Blocked, clearification required howto retrieve flood mask</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
   </numFmts>
-  <fonts count="17">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1414,6 +1422,12 @@
     <xf numFmtId="49" fontId="15" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
     <xf numFmtId="164" fontId="11" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1422,12 +1436,6 @@
     </xf>
     <xf numFmtId="164" fontId="11" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
@@ -1458,11 +1466,105 @@
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Hyperlink" xfId="2" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Pourcentage" xfId="1" builtinId="5"/>
+    <cellStyle name="Hyperlink" xfId="2"/>
+    <cellStyle name="Prozent" xfId="1" builtinId="5"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="405">
+  <dxfs count="413">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="6" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFC00000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="6" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFC00000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -6179,9 +6281,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Larissa">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -6219,9 +6321,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Larissa">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -6254,26 +6356,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -6306,26 +6391,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Larissa">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -6498,28 +6566,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I128"/>
   <sheetViews>
-    <sheetView topLeftCell="A44" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
+    <sheetView topLeftCell="A44" workbookViewId="0">
       <selection activeCell="A59" sqref="A59:XFD59"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.42578125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="2.44140625" style="1" customWidth="1"/>
     <col min="2" max="2" width="8" style="8" customWidth="1"/>
     <col min="3" max="3" width="55" style="23" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" style="1"/>
-    <col min="5" max="6" width="11.42578125" style="45"/>
-    <col min="7" max="7" width="19.42578125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="17.140625" style="2" customWidth="1"/>
-    <col min="9" max="9" width="87.5703125" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="11.42578125" style="1"/>
+    <col min="4" max="4" width="11.44140625" style="1"/>
+    <col min="5" max="6" width="11.44140625" style="45"/>
+    <col min="7" max="7" width="19.44140625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="17.109375" style="2" customWidth="1"/>
+    <col min="9" max="9" width="87.5546875" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="11.44140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="12" customHeight="1"/>
-    <row r="2" spans="1:9" ht="74.25" customHeight="1">
+    <row r="1" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:9" ht="74.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="10" t="s">
         <v>0</v>
       </c>
@@ -6527,13 +6595,13 @@
       <c r="D2" s="4"/>
       <c r="E2" s="56"/>
       <c r="F2" s="46"/>
-      <c r="G2" s="76" t="s">
+      <c r="G2" s="78" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="77"/>
-      <c r="I2" s="78"/>
-    </row>
-    <row r="3" spans="1:9" s="3" customFormat="1" ht="33" customHeight="1">
+      <c r="H2" s="79"/>
+      <c r="I2" s="80"/>
+    </row>
+    <row r="3" spans="1:9" s="3" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="41"/>
       <c r="B3" s="44" t="s">
         <v>2</v>
@@ -6560,7 +6628,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:9" s="27" customFormat="1" ht="29.25" customHeight="1">
+    <row r="4" spans="1:9" s="27" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="84" t="s">
         <v>10</v>
       </c>
@@ -6586,7 +6654,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:9" s="27" customFormat="1" ht="15" customHeight="1">
+    <row r="5" spans="1:9" s="27" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="85"/>
       <c r="C5" s="26" t="s">
         <v>17</v>
@@ -6608,7 +6676,7 @@
       </c>
       <c r="I5" s="26"/>
     </row>
-    <row r="6" spans="1:9" s="27" customFormat="1" ht="15" customHeight="1">
+    <row r="6" spans="1:9" s="27" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="85"/>
       <c r="C6" s="26" t="s">
         <v>23</v>
@@ -6630,7 +6698,7 @@
       </c>
       <c r="I6" s="26"/>
     </row>
-    <row r="7" spans="1:9" s="27" customFormat="1" ht="15" customHeight="1">
+    <row r="7" spans="1:9" s="27" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="85"/>
       <c r="C7" s="26"/>
       <c r="D7" s="11"/>
@@ -6640,7 +6708,7 @@
       <c r="H7" s="12"/>
       <c r="I7" s="26"/>
     </row>
-    <row r="8" spans="1:9" s="27" customFormat="1" ht="15" customHeight="1">
+    <row r="8" spans="1:9" s="27" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="85"/>
       <c r="C8" s="26"/>
       <c r="D8" s="11"/>
@@ -6650,7 +6718,7 @@
       <c r="H8" s="12"/>
       <c r="I8" s="26"/>
     </row>
-    <row r="9" spans="1:9" s="27" customFormat="1" ht="15" customHeight="1" thickBot="1">
+    <row r="9" spans="1:9" s="27" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B9" s="86"/>
       <c r="C9" s="38" t="s">
         <v>26</v>
@@ -6662,8 +6730,8 @@
       <c r="H9" s="17"/>
       <c r="I9" s="28"/>
     </row>
-    <row r="10" spans="1:9" ht="15" customHeight="1">
-      <c r="B10" s="79" t="s">
+    <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="76" t="s">
         <v>27</v>
       </c>
       <c r="C10" s="15" t="s">
@@ -6686,8 +6754,8 @@
       </c>
       <c r="I10" s="15"/>
     </row>
-    <row r="11" spans="1:9" ht="30.75" customHeight="1">
-      <c r="B11" s="79"/>
+    <row r="11" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="76"/>
       <c r="C11" s="23" t="s">
         <v>31</v>
       </c>
@@ -6710,8 +6778,8 @@
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="15" customHeight="1">
-      <c r="B12" s="79"/>
+    <row r="12" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="76"/>
       <c r="C12" s="25" t="s">
         <v>36</v>
       </c>
@@ -6734,8 +6802,8 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="15" customHeight="1">
-      <c r="B13" s="79"/>
+    <row r="13" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="76"/>
       <c r="C13" s="11" t="s">
         <v>40</v>
       </c>
@@ -6756,8 +6824,8 @@
       </c>
       <c r="I13" s="11"/>
     </row>
-    <row r="14" spans="1:9" ht="15" customHeight="1">
-      <c r="B14" s="79"/>
+    <row r="14" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="76"/>
       <c r="C14" s="11" t="s">
         <v>44</v>
       </c>
@@ -6780,8 +6848,8 @@
         <v>47</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="15" customHeight="1">
-      <c r="B15" s="79"/>
+    <row r="15" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="76"/>
       <c r="C15" s="29" t="s">
         <v>48</v>
       </c>
@@ -6804,8 +6872,8 @@
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="25.5" customHeight="1">
-      <c r="B16" s="79"/>
+    <row r="16" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="76"/>
       <c r="C16" s="29" t="s">
         <v>51</v>
       </c>
@@ -6826,8 +6894,8 @@
       </c>
       <c r="I16" s="29"/>
     </row>
-    <row r="17" spans="2:9" ht="15" customHeight="1">
-      <c r="B17" s="79"/>
+    <row r="17" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="76"/>
       <c r="C17" s="29" t="s">
         <v>53</v>
       </c>
@@ -6848,8 +6916,8 @@
       </c>
       <c r="I17" s="29"/>
     </row>
-    <row r="18" spans="2:9" ht="15" customHeight="1">
-      <c r="B18" s="79"/>
+    <row r="18" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="76"/>
       <c r="C18" s="29"/>
       <c r="D18" s="29"/>
       <c r="E18" s="29"/>
@@ -6858,8 +6926,8 @@
       <c r="H18" s="34"/>
       <c r="I18" s="29"/>
     </row>
-    <row r="19" spans="2:9" ht="15" customHeight="1">
-      <c r="B19" s="79"/>
+    <row r="19" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="76"/>
       <c r="C19" s="29"/>
       <c r="D19" s="29"/>
       <c r="E19" s="29"/>
@@ -6868,8 +6936,8 @@
       <c r="H19" s="34"/>
       <c r="I19" s="29"/>
     </row>
-    <row r="20" spans="2:9" ht="15" customHeight="1">
-      <c r="B20" s="79"/>
+    <row r="20" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="76"/>
       <c r="C20" s="29"/>
       <c r="D20" s="29"/>
       <c r="E20" s="29"/>
@@ -6878,8 +6946,8 @@
       <c r="H20" s="34"/>
       <c r="I20" s="29"/>
     </row>
-    <row r="21" spans="2:9" ht="15" customHeight="1" thickBot="1">
-      <c r="B21" s="80"/>
+    <row r="21" spans="2:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B21" s="77"/>
       <c r="C21" s="38" t="s">
         <v>26</v>
       </c>
@@ -6890,8 +6958,8 @@
       <c r="H21" s="14"/>
       <c r="I21" s="13"/>
     </row>
-    <row r="22" spans="2:9" ht="30" customHeight="1">
-      <c r="B22" s="79" t="s">
+    <row r="22" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="76" t="s">
         <v>54</v>
       </c>
       <c r="C22" s="15" t="s">
@@ -6914,8 +6982,8 @@
       </c>
       <c r="I22" s="15"/>
     </row>
-    <row r="23" spans="2:9" ht="43.5" customHeight="1">
-      <c r="B23" s="79"/>
+    <row r="23" spans="2:9" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="76"/>
       <c r="C23" s="11" t="s">
         <v>57</v>
       </c>
@@ -6936,8 +7004,8 @@
       </c>
       <c r="I23" s="11"/>
     </row>
-    <row r="24" spans="2:9" ht="26.25" customHeight="1">
-      <c r="B24" s="79"/>
+    <row r="24" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="76"/>
       <c r="C24" s="11" t="s">
         <v>58</v>
       </c>
@@ -6958,8 +7026,8 @@
       </c>
       <c r="I24" s="11"/>
     </row>
-    <row r="25" spans="2:9" ht="31.5" customHeight="1">
-      <c r="B25" s="79"/>
+    <row r="25" spans="2:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="76"/>
       <c r="C25" s="11" t="s">
         <v>59</v>
       </c>
@@ -6982,8 +7050,8 @@
         <v>61</v>
       </c>
     </row>
-    <row r="26" spans="2:9" ht="44.25" customHeight="1">
-      <c r="B26" s="79"/>
+    <row r="26" spans="2:9" ht="44.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="76"/>
       <c r="C26" s="65" t="s">
         <v>62</v>
       </c>
@@ -7006,8 +7074,8 @@
         <v>66</v>
       </c>
     </row>
-    <row r="27" spans="2:9" ht="44.25" customHeight="1">
-      <c r="B27" s="79"/>
+    <row r="27" spans="2:9" ht="44.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="76"/>
       <c r="C27" s="65"/>
       <c r="D27" s="65"/>
       <c r="E27" s="75"/>
@@ -7016,8 +7084,8 @@
       <c r="H27" s="74"/>
       <c r="I27" s="29"/>
     </row>
-    <row r="28" spans="2:9" ht="15" customHeight="1">
-      <c r="B28" s="79"/>
+    <row r="28" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="76"/>
       <c r="C28" s="29"/>
       <c r="D28" s="29"/>
       <c r="E28" s="22"/>
@@ -7026,8 +7094,8 @@
       <c r="H28" s="34"/>
       <c r="I28" s="29"/>
     </row>
-    <row r="29" spans="2:9" ht="16.5" customHeight="1">
-      <c r="B29" s="79"/>
+    <row r="29" spans="2:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="76"/>
       <c r="C29" s="29"/>
       <c r="D29" s="29"/>
       <c r="E29" s="22"/>
@@ -7036,8 +7104,8 @@
       <c r="H29" s="34"/>
       <c r="I29" s="29"/>
     </row>
-    <row r="30" spans="2:9" ht="15" customHeight="1" thickBot="1">
-      <c r="B30" s="80"/>
+    <row r="30" spans="2:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B30" s="77"/>
       <c r="C30" s="38" t="s">
         <v>26</v>
       </c>
@@ -7048,8 +7116,8 @@
       <c r="H30" s="17"/>
       <c r="I30" s="13"/>
     </row>
-    <row r="31" spans="2:9" ht="24.75" customHeight="1">
-      <c r="B31" s="79" t="s">
+    <row r="31" spans="2:9" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="76" t="s">
         <v>67</v>
       </c>
       <c r="C31" s="15" t="s">
@@ -7074,8 +7142,8 @@
         <v>71</v>
       </c>
     </row>
-    <row r="32" spans="2:9" ht="15" customHeight="1">
-      <c r="B32" s="79"/>
+    <row r="32" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="76"/>
       <c r="C32" s="11" t="s">
         <v>72</v>
       </c>
@@ -7098,8 +7166,8 @@
         <v>74</v>
       </c>
     </row>
-    <row r="33" spans="2:9" ht="41.25" customHeight="1">
-      <c r="B33" s="79"/>
+    <row r="33" spans="2:9" ht="41.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="76"/>
       <c r="C33" s="11" t="s">
         <v>75</v>
       </c>
@@ -7122,8 +7190,8 @@
         <v>77</v>
       </c>
     </row>
-    <row r="34" spans="2:9" ht="63" customHeight="1">
-      <c r="B34" s="79"/>
+    <row r="34" spans="2:9" ht="63" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="76"/>
       <c r="C34" s="29" t="s">
         <v>78</v>
       </c>
@@ -7146,8 +7214,8 @@
         <v>74</v>
       </c>
     </row>
-    <row r="35" spans="2:9" ht="168.75" customHeight="1">
-      <c r="B35" s="79"/>
+    <row r="35" spans="2:9" ht="168.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B35" s="76"/>
       <c r="C35" s="29" t="s">
         <v>80</v>
       </c>
@@ -7170,8 +7238,8 @@
         <v>82</v>
       </c>
     </row>
-    <row r="36" spans="2:9" ht="74.25" customHeight="1">
-      <c r="B36" s="79"/>
+    <row r="36" spans="2:9" ht="74.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B36" s="76"/>
       <c r="C36" s="67" t="s">
         <v>83</v>
       </c>
@@ -7194,8 +7262,8 @@
         <v>74</v>
       </c>
     </row>
-    <row r="37" spans="2:9" ht="16.5" customHeight="1">
-      <c r="B37" s="79"/>
+    <row r="37" spans="2:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B37" s="76"/>
       <c r="C37" s="39" t="s">
         <v>85</v>
       </c>
@@ -7216,8 +7284,8 @@
       </c>
       <c r="I37" s="11"/>
     </row>
-    <row r="38" spans="2:9" ht="16.5" customHeight="1">
-      <c r="B38" s="79"/>
+    <row r="38" spans="2:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B38" s="76"/>
       <c r="C38" s="54" t="s">
         <v>87</v>
       </c>
@@ -7238,8 +7306,8 @@
       </c>
       <c r="I38" s="29"/>
     </row>
-    <row r="39" spans="2:9" ht="16.5" customHeight="1">
-      <c r="B39" s="79"/>
+    <row r="39" spans="2:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B39" s="76"/>
       <c r="C39" s="54"/>
       <c r="D39" s="29"/>
       <c r="E39" s="29"/>
@@ -7248,8 +7316,8 @@
       <c r="H39" s="30"/>
       <c r="I39" s="29"/>
     </row>
-    <row r="40" spans="2:9" ht="16.5" customHeight="1">
-      <c r="B40" s="79"/>
+    <row r="40" spans="2:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B40" s="76"/>
       <c r="C40" s="54"/>
       <c r="D40" s="29"/>
       <c r="E40" s="29"/>
@@ -7258,8 +7326,8 @@
       <c r="H40" s="30"/>
       <c r="I40" s="29"/>
     </row>
-    <row r="41" spans="2:9" ht="16.5" customHeight="1">
-      <c r="B41" s="79"/>
+    <row r="41" spans="2:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B41" s="76"/>
       <c r="C41" s="35"/>
       <c r="D41" s="29"/>
       <c r="E41" s="29"/>
@@ -7268,8 +7336,8 @@
       <c r="H41" s="30"/>
       <c r="I41" s="29"/>
     </row>
-    <row r="42" spans="2:9" ht="16.5" customHeight="1" thickBot="1">
-      <c r="B42" s="80"/>
+    <row r="42" spans="2:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B42" s="77"/>
       <c r="C42" s="38" t="s">
         <v>26</v>
       </c>
@@ -7280,8 +7348,8 @@
       <c r="H42" s="7"/>
       <c r="I42" s="7"/>
     </row>
-    <row r="43" spans="2:9" ht="40.5" customHeight="1">
-      <c r="B43" s="79" t="s">
+    <row r="43" spans="2:9" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B43" s="76" t="s">
         <v>90</v>
       </c>
       <c r="C43" s="15" t="s">
@@ -7306,8 +7374,8 @@
         <v>94</v>
       </c>
     </row>
-    <row r="44" spans="2:9" ht="25.5">
-      <c r="B44" s="79"/>
+    <row r="44" spans="2:9" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="B44" s="76"/>
       <c r="C44" s="11" t="s">
         <v>95</v>
       </c>
@@ -7330,8 +7398,8 @@
         <v>96</v>
       </c>
     </row>
-    <row r="45" spans="2:9" ht="25.5">
-      <c r="B45" s="79"/>
+    <row r="45" spans="2:9" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="B45" s="76"/>
       <c r="C45" s="55" t="s">
         <v>97</v>
       </c>
@@ -7354,8 +7422,8 @@
         <v>101</v>
       </c>
     </row>
-    <row r="46" spans="2:9" ht="25.5">
-      <c r="B46" s="79"/>
+    <row r="46" spans="2:9" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="B46" s="76"/>
       <c r="C46" s="40" t="s">
         <v>102</v>
       </c>
@@ -7376,8 +7444,8 @@
       </c>
       <c r="I46" s="11"/>
     </row>
-    <row r="47" spans="2:9" ht="25.5">
-      <c r="B47" s="79"/>
+    <row r="47" spans="2:9" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="B47" s="76"/>
       <c r="C47" s="40" t="s">
         <v>104</v>
       </c>
@@ -7398,8 +7466,8 @@
       </c>
       <c r="I47" s="11"/>
     </row>
-    <row r="48" spans="2:9" ht="38.25">
-      <c r="B48" s="79"/>
+    <row r="48" spans="2:9" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="B48" s="76"/>
       <c r="C48" s="11" t="s">
         <v>107</v>
       </c>
@@ -7420,8 +7488,8 @@
       </c>
       <c r="I48" s="11"/>
     </row>
-    <row r="49" spans="2:9" ht="25.5">
-      <c r="B49" s="79"/>
+    <row r="49" spans="2:9" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="B49" s="76"/>
       <c r="C49" s="11" t="s">
         <v>109</v>
       </c>
@@ -7444,8 +7512,8 @@
         <v>110</v>
       </c>
     </row>
-    <row r="50" spans="2:9" ht="38.25">
-      <c r="B50" s="79"/>
+    <row r="50" spans="2:9" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="B50" s="76"/>
       <c r="C50" s="29" t="s">
         <v>111</v>
       </c>
@@ -7466,8 +7534,8 @@
       </c>
       <c r="I50" s="29"/>
     </row>
-    <row r="51" spans="2:9">
-      <c r="B51" s="79"/>
+    <row r="51" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B51" s="76"/>
       <c r="C51" s="29"/>
       <c r="D51" s="29"/>
       <c r="E51" s="70"/>
@@ -7476,8 +7544,8 @@
       <c r="H51" s="30"/>
       <c r="I51" s="29"/>
     </row>
-    <row r="52" spans="2:9">
-      <c r="B52" s="79"/>
+    <row r="52" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B52" s="76"/>
       <c r="C52" s="29"/>
       <c r="D52" s="29"/>
       <c r="E52" s="70"/>
@@ -7486,8 +7554,8 @@
       <c r="H52" s="30"/>
       <c r="I52" s="29"/>
     </row>
-    <row r="53" spans="2:9">
-      <c r="B53" s="79"/>
+    <row r="53" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B53" s="76"/>
       <c r="C53" s="29"/>
       <c r="D53" s="29"/>
       <c r="E53" s="70"/>
@@ -7496,8 +7564,8 @@
       <c r="H53" s="30"/>
       <c r="I53" s="29"/>
     </row>
-    <row r="54" spans="2:9" ht="13.5" thickBot="1">
-      <c r="B54" s="80"/>
+    <row r="54" spans="2:9" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B54" s="77"/>
       <c r="C54" s="38" t="s">
         <v>26</v>
       </c>
@@ -7508,8 +7576,8 @@
       <c r="H54" s="17"/>
       <c r="I54" s="13"/>
     </row>
-    <row r="55" spans="2:9" ht="40.5" customHeight="1">
-      <c r="B55" s="79" t="s">
+    <row r="55" spans="2:9" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B55" s="76" t="s">
         <v>113</v>
       </c>
       <c r="C55" s="15" t="s">
@@ -7532,8 +7600,8 @@
       </c>
       <c r="I55" s="15"/>
     </row>
-    <row r="56" spans="2:9" ht="47.25" customHeight="1">
-      <c r="B56" s="79"/>
+    <row r="56" spans="2:9" ht="47.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B56" s="76"/>
       <c r="C56" s="11" t="s">
         <v>116</v>
       </c>
@@ -7554,8 +7622,8 @@
       </c>
       <c r="I56" s="11"/>
     </row>
-    <row r="57" spans="2:9" ht="40.5" customHeight="1">
-      <c r="B57" s="79"/>
+    <row r="57" spans="2:9" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B57" s="76"/>
       <c r="C57" s="25" t="s">
         <v>117</v>
       </c>
@@ -7576,8 +7644,8 @@
       </c>
       <c r="I57" s="11"/>
     </row>
-    <row r="58" spans="2:9" ht="18" customHeight="1">
-      <c r="B58" s="79"/>
+    <row r="58" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B58" s="76"/>
       <c r="C58" s="25"/>
       <c r="D58" s="11"/>
       <c r="E58" s="49"/>
@@ -7586,8 +7654,8 @@
       <c r="H58" s="19"/>
       <c r="I58" s="11"/>
     </row>
-    <row r="59" spans="2:9" ht="18" customHeight="1">
-      <c r="B59" s="79"/>
+    <row r="59" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B59" s="76"/>
       <c r="C59" s="25"/>
       <c r="D59" s="11"/>
       <c r="E59" s="49"/>
@@ -7596,8 +7664,8 @@
       <c r="H59" s="19"/>
       <c r="I59" s="11"/>
     </row>
-    <row r="60" spans="2:9" ht="14.25" customHeight="1">
-      <c r="B60" s="79"/>
+    <row r="60" spans="2:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B60" s="76"/>
       <c r="C60" s="25"/>
       <c r="D60" s="11"/>
       <c r="E60" s="49"/>
@@ -7606,8 +7674,8 @@
       <c r="H60" s="72"/>
       <c r="I60" s="11"/>
     </row>
-    <row r="61" spans="2:9" ht="13.5" thickBot="1">
-      <c r="B61" s="80"/>
+    <row r="61" spans="2:9" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B61" s="77"/>
       <c r="C61" s="38" t="s">
         <v>26</v>
       </c>
@@ -7618,8 +7686,8 @@
       <c r="H61" s="17"/>
       <c r="I61" s="13"/>
     </row>
-    <row r="62" spans="2:9" ht="25.5" customHeight="1">
-      <c r="B62" s="79" t="s">
+    <row r="62" spans="2:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B62" s="76" t="s">
         <v>119</v>
       </c>
       <c r="C62" s="15" t="s">
@@ -7642,8 +7710,8 @@
       </c>
       <c r="I62" s="15"/>
     </row>
-    <row r="63" spans="2:9">
-      <c r="B63" s="79"/>
+    <row r="63" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B63" s="76"/>
       <c r="C63" s="11"/>
       <c r="D63" s="11"/>
       <c r="E63" s="11"/>
@@ -7652,8 +7720,8 @@
       <c r="H63" s="19"/>
       <c r="I63" s="11"/>
     </row>
-    <row r="64" spans="2:9">
-      <c r="B64" s="79"/>
+    <row r="64" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B64" s="76"/>
       <c r="C64" s="11"/>
       <c r="D64" s="11"/>
       <c r="E64" s="11"/>
@@ -7662,8 +7730,8 @@
       <c r="H64" s="19"/>
       <c r="I64" s="11"/>
     </row>
-    <row r="65" spans="2:9">
-      <c r="B65" s="79"/>
+    <row r="65" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B65" s="76"/>
       <c r="C65" s="11"/>
       <c r="D65" s="11"/>
       <c r="E65" s="11"/>
@@ -7672,8 +7740,8 @@
       <c r="H65" s="19"/>
       <c r="I65" s="11"/>
     </row>
-    <row r="66" spans="2:9" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B66" s="80"/>
+    <row r="66" spans="2:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B66" s="77"/>
       <c r="C66" s="38" t="s">
         <v>26</v>
       </c>
@@ -7684,7 +7752,7 @@
       <c r="H66" s="17"/>
       <c r="I66" s="13"/>
     </row>
-    <row r="67" spans="2:9" ht="15" customHeight="1">
+    <row r="67" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B67" s="87" t="s">
         <v>123</v>
       </c>
@@ -7708,8 +7776,8 @@
       </c>
       <c r="I67" s="15"/>
     </row>
-    <row r="68" spans="2:9" ht="25.5">
-      <c r="B68" s="79"/>
+    <row r="68" spans="2:9" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="B68" s="76"/>
       <c r="C68" s="11" t="s">
         <v>126</v>
       </c>
@@ -7732,8 +7800,8 @@
         <v>128</v>
       </c>
     </row>
-    <row r="69" spans="2:9">
-      <c r="B69" s="79"/>
+    <row r="69" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B69" s="76"/>
       <c r="C69" s="11" t="s">
         <v>129</v>
       </c>
@@ -7754,8 +7822,8 @@
       </c>
       <c r="I69" s="11"/>
     </row>
-    <row r="70" spans="2:9" ht="38.25">
-      <c r="B70" s="79"/>
+    <row r="70" spans="2:9" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="B70" s="76"/>
       <c r="C70" s="11" t="s">
         <v>130</v>
       </c>
@@ -7778,8 +7846,8 @@
         <v>132</v>
       </c>
     </row>
-    <row r="71" spans="2:9" ht="42" customHeight="1">
-      <c r="B71" s="79"/>
+    <row r="71" spans="2:9" ht="42" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B71" s="76"/>
       <c r="C71" s="40" t="s">
         <v>133</v>
       </c>
@@ -7802,8 +7870,8 @@
         <v>134</v>
       </c>
     </row>
-    <row r="72" spans="2:9" ht="25.5">
-      <c r="B72" s="79"/>
+    <row r="72" spans="2:9" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="B72" s="76"/>
       <c r="C72" s="11" t="s">
         <v>135</v>
       </c>
@@ -7826,8 +7894,8 @@
         <v>137</v>
       </c>
     </row>
-    <row r="73" spans="2:9" ht="38.25">
-      <c r="B73" s="79"/>
+    <row r="73" spans="2:9" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="B73" s="76"/>
       <c r="C73" s="11" t="s">
         <v>138</v>
       </c>
@@ -7850,8 +7918,8 @@
         <v>141</v>
       </c>
     </row>
-    <row r="74" spans="2:9" ht="25.5">
-      <c r="B74" s="79"/>
+    <row r="74" spans="2:9" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="B74" s="76"/>
       <c r="C74" s="25" t="s">
         <v>142</v>
       </c>
@@ -7874,8 +7942,8 @@
         <v>144</v>
       </c>
     </row>
-    <row r="75" spans="2:9">
-      <c r="B75" s="79"/>
+    <row r="75" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B75" s="76"/>
       <c r="C75" s="57"/>
       <c r="D75" s="11"/>
       <c r="E75" s="49"/>
@@ -7884,8 +7952,8 @@
       <c r="H75" s="19"/>
       <c r="I75" s="29"/>
     </row>
-    <row r="76" spans="2:9">
-      <c r="B76" s="79"/>
+    <row r="76" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B76" s="76"/>
       <c r="C76" s="29"/>
       <c r="D76" s="11"/>
       <c r="E76" s="11"/>
@@ -7894,8 +7962,8 @@
       <c r="H76" s="19"/>
       <c r="I76" s="29"/>
     </row>
-    <row r="77" spans="2:9">
-      <c r="B77" s="79"/>
+    <row r="77" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B77" s="76"/>
       <c r="C77" s="29"/>
       <c r="D77" s="11"/>
       <c r="E77" s="11"/>
@@ -7904,7 +7972,7 @@
       <c r="H77" s="19"/>
       <c r="I77" s="29"/>
     </row>
-    <row r="78" spans="2:9" ht="13.5" thickBot="1">
+    <row r="78" spans="2:9" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B78" s="81"/>
       <c r="C78" s="38" t="s">
         <v>26</v>
@@ -7916,7 +7984,7 @@
       <c r="H78" s="37"/>
       <c r="I78" s="13"/>
     </row>
-    <row r="79" spans="2:9" ht="15" customHeight="1">
+    <row r="79" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B79" s="88" t="s">
         <v>145</v>
       </c>
@@ -7940,8 +8008,8 @@
       </c>
       <c r="I79" s="15"/>
     </row>
-    <row r="80" spans="2:9">
-      <c r="B80" s="79"/>
+    <row r="80" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B80" s="76"/>
       <c r="C80" s="11"/>
       <c r="D80" s="11"/>
       <c r="E80" s="11"/>
@@ -7950,8 +8018,8 @@
       <c r="H80" s="19"/>
       <c r="I80" s="11"/>
     </row>
-    <row r="81" spans="2:9">
-      <c r="B81" s="79"/>
+    <row r="81" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B81" s="76"/>
       <c r="C81" s="11"/>
       <c r="D81" s="11"/>
       <c r="E81" s="11"/>
@@ -7960,8 +8028,8 @@
       <c r="H81" s="19"/>
       <c r="I81" s="11"/>
     </row>
-    <row r="82" spans="2:9">
-      <c r="B82" s="79"/>
+    <row r="82" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B82" s="76"/>
       <c r="C82" s="11"/>
       <c r="D82" s="11"/>
       <c r="E82" s="11"/>
@@ -7970,8 +8038,8 @@
       <c r="H82" s="19"/>
       <c r="I82" s="11"/>
     </row>
-    <row r="83" spans="2:9">
-      <c r="B83" s="79"/>
+    <row r="83" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B83" s="76"/>
       <c r="C83" s="11"/>
       <c r="D83" s="11"/>
       <c r="E83" s="11"/>
@@ -7980,8 +8048,8 @@
       <c r="H83" s="19"/>
       <c r="I83" s="11"/>
     </row>
-    <row r="84" spans="2:9" ht="13.5" thickBot="1">
-      <c r="B84" s="80"/>
+    <row r="84" spans="2:9" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B84" s="77"/>
       <c r="C84" s="38" t="s">
         <v>26</v>
       </c>
@@ -7992,8 +8060,8 @@
       <c r="H84" s="17"/>
       <c r="I84" s="13"/>
     </row>
-    <row r="85" spans="2:9" ht="15" customHeight="1">
-      <c r="B85" s="79" t="s">
+    <row r="85" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B85" s="76" t="s">
         <v>148</v>
       </c>
       <c r="C85" s="15"/>
@@ -8004,8 +8072,8 @@
       <c r="H85" s="18"/>
       <c r="I85" s="15"/>
     </row>
-    <row r="86" spans="2:9">
-      <c r="B86" s="79"/>
+    <row r="86" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B86" s="76"/>
       <c r="C86" s="11"/>
       <c r="D86" s="11"/>
       <c r="E86" s="11"/>
@@ -8014,8 +8082,8 @@
       <c r="H86" s="19"/>
       <c r="I86" s="11"/>
     </row>
-    <row r="87" spans="2:9">
-      <c r="B87" s="79"/>
+    <row r="87" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B87" s="76"/>
       <c r="C87" s="11"/>
       <c r="D87" s="11"/>
       <c r="E87" s="11"/>
@@ -8024,8 +8092,8 @@
       <c r="H87" s="19"/>
       <c r="I87" s="11"/>
     </row>
-    <row r="88" spans="2:9">
-      <c r="B88" s="79"/>
+    <row r="88" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B88" s="76"/>
       <c r="C88" s="11"/>
       <c r="D88" s="11"/>
       <c r="E88" s="11"/>
@@ -8034,8 +8102,8 @@
       <c r="H88" s="19"/>
       <c r="I88" s="11"/>
     </row>
-    <row r="89" spans="2:9" ht="13.5" thickBot="1">
-      <c r="B89" s="80"/>
+    <row r="89" spans="2:9" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B89" s="77"/>
       <c r="C89" s="38" t="s">
         <v>26</v>
       </c>
@@ -8046,8 +8114,8 @@
       <c r="H89" s="17"/>
       <c r="I89" s="13"/>
     </row>
-    <row r="90" spans="2:9" ht="27.75" customHeight="1">
-      <c r="B90" s="79" t="s">
+    <row r="90" spans="2:9" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B90" s="76" t="s">
         <v>149</v>
       </c>
       <c r="C90" s="11" t="s">
@@ -8072,8 +8140,8 @@
         <v>152</v>
       </c>
     </row>
-    <row r="91" spans="2:9" ht="15.75" customHeight="1">
-      <c r="B91" s="79"/>
+    <row r="91" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B91" s="76"/>
       <c r="C91" s="11"/>
       <c r="D91" s="11"/>
       <c r="E91" s="11"/>
@@ -8082,8 +8150,8 @@
       <c r="H91" s="19"/>
       <c r="I91" s="11"/>
     </row>
-    <row r="92" spans="2:9" ht="15.75" customHeight="1">
-      <c r="B92" s="79"/>
+    <row r="92" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B92" s="76"/>
       <c r="C92" s="11"/>
       <c r="D92" s="11"/>
       <c r="E92" s="11"/>
@@ -8092,8 +8160,8 @@
       <c r="H92" s="19"/>
       <c r="I92" s="11"/>
     </row>
-    <row r="93" spans="2:9" ht="15.75" customHeight="1">
-      <c r="B93" s="79"/>
+    <row r="93" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B93" s="76"/>
       <c r="C93" s="11"/>
       <c r="D93" s="11"/>
       <c r="E93" s="11"/>
@@ -8102,8 +8170,8 @@
       <c r="H93" s="19"/>
       <c r="I93" s="11"/>
     </row>
-    <row r="94" spans="2:9" ht="15.75" customHeight="1">
-      <c r="B94" s="79"/>
+    <row r="94" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B94" s="76"/>
       <c r="C94" s="11"/>
       <c r="D94" s="11"/>
       <c r="E94" s="11"/>
@@ -8112,8 +8180,8 @@
       <c r="H94" s="19"/>
       <c r="I94" s="11"/>
     </row>
-    <row r="95" spans="2:9" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B95" s="80"/>
+    <row r="95" spans="2:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B95" s="77"/>
       <c r="C95" s="38" t="s">
         <v>26</v>
       </c>
@@ -8124,8 +8192,8 @@
       <c r="H95" s="17"/>
       <c r="I95" s="13"/>
     </row>
-    <row r="96" spans="2:9" ht="15" customHeight="1">
-      <c r="B96" s="79" t="s">
+    <row r="96" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B96" s="76" t="s">
         <v>153</v>
       </c>
       <c r="C96" s="15" t="s">
@@ -8150,8 +8218,8 @@
         <v>155</v>
       </c>
     </row>
-    <row r="97" spans="2:9">
-      <c r="B97" s="79"/>
+    <row r="97" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B97" s="76"/>
       <c r="C97" s="11"/>
       <c r="D97" s="11"/>
       <c r="E97" s="11"/>
@@ -8160,8 +8228,8 @@
       <c r="H97" s="19"/>
       <c r="I97" s="11"/>
     </row>
-    <row r="98" spans="2:9">
-      <c r="B98" s="79"/>
+    <row r="98" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B98" s="76"/>
       <c r="C98" s="11"/>
       <c r="D98" s="11"/>
       <c r="E98" s="11"/>
@@ -8170,8 +8238,8 @@
       <c r="H98" s="19"/>
       <c r="I98" s="11"/>
     </row>
-    <row r="99" spans="2:9">
-      <c r="B99" s="79"/>
+    <row r="99" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B99" s="76"/>
       <c r="C99" s="11"/>
       <c r="D99" s="11"/>
       <c r="E99" s="11"/>
@@ -8180,8 +8248,8 @@
       <c r="H99" s="19"/>
       <c r="I99" s="11"/>
     </row>
-    <row r="100" spans="2:9">
-      <c r="B100" s="79"/>
+    <row r="100" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B100" s="76"/>
       <c r="C100" s="11"/>
       <c r="D100" s="11"/>
       <c r="E100" s="11"/>
@@ -8190,8 +8258,8 @@
       <c r="H100" s="19"/>
       <c r="I100" s="11"/>
     </row>
-    <row r="101" spans="2:9" ht="13.5" thickBot="1">
-      <c r="B101" s="80"/>
+    <row r="101" spans="2:9" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B101" s="77"/>
       <c r="C101" s="38" t="s">
         <v>26</v>
       </c>
@@ -8202,8 +8270,8 @@
       <c r="H101" s="17"/>
       <c r="I101" s="13"/>
     </row>
-    <row r="102" spans="2:9" ht="15" customHeight="1">
-      <c r="B102" s="79" t="s">
+    <row r="102" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B102" s="76" t="s">
         <v>156</v>
       </c>
       <c r="C102" s="15"/>
@@ -8214,8 +8282,8 @@
       <c r="H102" s="18"/>
       <c r="I102" s="15"/>
     </row>
-    <row r="103" spans="2:9">
-      <c r="B103" s="79"/>
+    <row r="103" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B103" s="76"/>
       <c r="C103" s="11"/>
       <c r="D103" s="11"/>
       <c r="E103" s="11"/>
@@ -8224,8 +8292,8 @@
       <c r="H103" s="19"/>
       <c r="I103" s="11"/>
     </row>
-    <row r="104" spans="2:9">
-      <c r="B104" s="79"/>
+    <row r="104" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B104" s="76"/>
       <c r="C104" s="11"/>
       <c r="D104" s="11"/>
       <c r="E104" s="11"/>
@@ -8234,8 +8302,8 @@
       <c r="H104" s="19"/>
       <c r="I104" s="11"/>
     </row>
-    <row r="105" spans="2:9">
-      <c r="B105" s="79"/>
+    <row r="105" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B105" s="76"/>
       <c r="C105" s="11"/>
       <c r="D105" s="11"/>
       <c r="E105" s="11"/>
@@ -8244,8 +8312,8 @@
       <c r="H105" s="19"/>
       <c r="I105" s="11"/>
     </row>
-    <row r="106" spans="2:9">
-      <c r="B106" s="79"/>
+    <row r="106" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B106" s="76"/>
       <c r="C106" s="11"/>
       <c r="D106" s="11"/>
       <c r="E106" s="11"/>
@@ -8254,8 +8322,8 @@
       <c r="H106" s="19"/>
       <c r="I106" s="11"/>
     </row>
-    <row r="107" spans="2:9" ht="13.5" thickBot="1">
-      <c r="B107" s="80"/>
+    <row r="107" spans="2:9" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B107" s="77"/>
       <c r="C107" s="38" t="s">
         <v>26</v>
       </c>
@@ -8266,8 +8334,8 @@
       <c r="H107" s="17"/>
       <c r="I107" s="13"/>
     </row>
-    <row r="108" spans="2:9" ht="15" customHeight="1">
-      <c r="B108" s="79" t="s">
+    <row r="108" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B108" s="76" t="s">
         <v>157</v>
       </c>
       <c r="C108" s="15" t="s">
@@ -8292,8 +8360,8 @@
         <v>160</v>
       </c>
     </row>
-    <row r="109" spans="2:9">
-      <c r="B109" s="79"/>
+    <row r="109" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B109" s="76"/>
       <c r="C109" s="11"/>
       <c r="D109" s="11"/>
       <c r="E109" s="11"/>
@@ -8302,8 +8370,8 @@
       <c r="H109" s="19"/>
       <c r="I109" s="11"/>
     </row>
-    <row r="110" spans="2:9">
-      <c r="B110" s="79"/>
+    <row r="110" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B110" s="76"/>
       <c r="C110" s="11"/>
       <c r="D110" s="11"/>
       <c r="E110" s="11"/>
@@ -8312,8 +8380,8 @@
       <c r="H110" s="19"/>
       <c r="I110" s="11"/>
     </row>
-    <row r="111" spans="2:9">
-      <c r="B111" s="79"/>
+    <row r="111" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B111" s="76"/>
       <c r="C111" s="11"/>
       <c r="D111" s="11"/>
       <c r="E111" s="11"/>
@@ -8322,8 +8390,8 @@
       <c r="H111" s="19"/>
       <c r="I111" s="11"/>
     </row>
-    <row r="112" spans="2:9">
-      <c r="B112" s="79"/>
+    <row r="112" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B112" s="76"/>
       <c r="C112" s="11"/>
       <c r="D112" s="11"/>
       <c r="E112" s="11"/>
@@ -8332,8 +8400,8 @@
       <c r="H112" s="19"/>
       <c r="I112" s="11"/>
     </row>
-    <row r="113" spans="2:9" ht="13.5" thickBot="1">
-      <c r="B113" s="80"/>
+    <row r="113" spans="2:9" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B113" s="77"/>
       <c r="C113" s="38" t="s">
         <v>26</v>
       </c>
@@ -8344,8 +8412,8 @@
       <c r="H113" s="17"/>
       <c r="I113" s="13"/>
     </row>
-    <row r="114" spans="2:9" ht="81.75" customHeight="1">
-      <c r="B114" s="79" t="s">
+    <row r="114" spans="2:9" ht="81.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B114" s="76" t="s">
         <v>161</v>
       </c>
       <c r="C114" s="15" t="s">
@@ -8370,8 +8438,8 @@
         <v>164</v>
       </c>
     </row>
-    <row r="115" spans="2:9">
-      <c r="B115" s="79"/>
+    <row r="115" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B115" s="76"/>
       <c r="C115" s="11" t="s">
         <v>165</v>
       </c>
@@ -8392,8 +8460,8 @@
       </c>
       <c r="I115" s="11"/>
     </row>
-    <row r="116" spans="2:9">
-      <c r="B116" s="79"/>
+    <row r="116" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B116" s="76"/>
       <c r="C116" s="11"/>
       <c r="D116" s="11"/>
       <c r="E116" s="15"/>
@@ -8402,8 +8470,8 @@
       <c r="H116" s="19"/>
       <c r="I116" s="11"/>
     </row>
-    <row r="117" spans="2:9">
-      <c r="B117" s="79"/>
+    <row r="117" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B117" s="76"/>
       <c r="C117" s="11"/>
       <c r="D117" s="11"/>
       <c r="E117" s="11"/>
@@ -8412,8 +8480,8 @@
       <c r="H117" s="19"/>
       <c r="I117" s="11"/>
     </row>
-    <row r="118" spans="2:9">
-      <c r="B118" s="79"/>
+    <row r="118" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B118" s="76"/>
       <c r="C118" s="11"/>
       <c r="D118" s="11"/>
       <c r="E118" s="11"/>
@@ -8422,8 +8490,8 @@
       <c r="H118" s="19"/>
       <c r="I118" s="11"/>
     </row>
-    <row r="119" spans="2:9" ht="13.5" thickBot="1">
-      <c r="B119" s="80"/>
+    <row r="119" spans="2:9" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B119" s="77"/>
       <c r="C119" s="38" t="s">
         <v>26</v>
       </c>
@@ -8434,7 +8502,7 @@
       <c r="H119" s="17"/>
       <c r="I119" s="13"/>
     </row>
-    <row r="120" spans="2:9" ht="15" customHeight="1">
+    <row r="120" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B120" s="81" t="s">
         <v>166</v>
       </c>
@@ -8446,7 +8514,7 @@
       <c r="H120" s="18"/>
       <c r="I120" s="15"/>
     </row>
-    <row r="121" spans="2:9">
+    <row r="121" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B121" s="82"/>
       <c r="C121" s="11"/>
       <c r="D121" s="11"/>
@@ -8456,7 +8524,7 @@
       <c r="H121" s="19"/>
       <c r="I121" s="11"/>
     </row>
-    <row r="122" spans="2:9">
+    <row r="122" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B122" s="82"/>
       <c r="C122" s="11"/>
       <c r="D122" s="11"/>
@@ -8466,7 +8534,7 @@
       <c r="H122" s="19"/>
       <c r="I122" s="11"/>
     </row>
-    <row r="123" spans="2:9">
+    <row r="123" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B123" s="82"/>
       <c r="C123" s="11"/>
       <c r="D123" s="11"/>
@@ -8476,7 +8544,7 @@
       <c r="H123" s="19"/>
       <c r="I123" s="11"/>
     </row>
-    <row r="124" spans="2:9">
+    <row r="124" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B124" s="82"/>
       <c r="C124" s="11"/>
       <c r="D124" s="11"/>
@@ -8486,7 +8554,7 @@
       <c r="H124" s="19"/>
       <c r="I124" s="11"/>
     </row>
-    <row r="125" spans="2:9" ht="13.5" thickBot="1">
+    <row r="125" spans="2:9" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B125" s="83"/>
       <c r="C125" s="38" t="s">
         <v>26</v>
@@ -8498,7 +8566,7 @@
       <c r="H125" s="17"/>
       <c r="I125" s="13"/>
     </row>
-    <row r="126" spans="2:9">
+    <row r="126" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B126" s="9"/>
       <c r="C126" s="20"/>
       <c r="D126" s="20"/>
@@ -8508,7 +8576,7 @@
       <c r="H126" s="21"/>
       <c r="I126" s="20"/>
     </row>
-    <row r="127" spans="2:9">
+    <row r="127" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C127" s="20"/>
       <c r="D127" s="20"/>
       <c r="E127" s="50"/>
@@ -8517,17 +8585,12 @@
       <c r="H127" s="21"/>
       <c r="I127" s="20"/>
     </row>
-    <row r="128" spans="2:9">
+    <row r="128" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B128" s="9"/>
     </row>
   </sheetData>
-  <autoFilter ref="B3:I125" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="B3:I125"/>
   <mergeCells count="17">
-    <mergeCell ref="B43:B54"/>
-    <mergeCell ref="G2:I2"/>
-    <mergeCell ref="B102:B107"/>
-    <mergeCell ref="B108:B113"/>
-    <mergeCell ref="B114:B119"/>
     <mergeCell ref="B120:B125"/>
     <mergeCell ref="B90:B95"/>
     <mergeCell ref="B4:B9"/>
@@ -8540,333 +8603,338 @@
     <mergeCell ref="B22:B30"/>
     <mergeCell ref="B31:B42"/>
     <mergeCell ref="B55:B61"/>
+    <mergeCell ref="B43:B54"/>
+    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="B102:B107"/>
+    <mergeCell ref="B108:B113"/>
+    <mergeCell ref="B114:B119"/>
   </mergeCells>
   <conditionalFormatting sqref="G96:G100 G89">
-    <cfRule type="containsText" dxfId="404" priority="92" operator="containsText" text="Pending">
+    <cfRule type="containsText" dxfId="412" priority="92" operator="containsText" text="Pending">
       <formula>NOT(ISERROR(SEARCH("Pending",G89)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1 H25:H28 H73 H43 H78:H90 H13:H23 H10:H11 H48:H56 H30:H41 H61:H71 H96:H1048576">
-    <cfRule type="cellIs" dxfId="403" priority="88" operator="equal">
+    <cfRule type="cellIs" dxfId="411" priority="88" operator="equal">
       <formula>"Due/Overdue"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="402" priority="89" operator="equal">
+    <cfRule type="cellIs" dxfId="410" priority="89" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="401" priority="90" operator="equal">
+    <cfRule type="cellIs" dxfId="409" priority="90" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="400" priority="91" operator="equal">
+    <cfRule type="cellIs" dxfId="408" priority="91" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D3 D25:D28 D30:D41 D73 D43 D96:D1048576 D78:D90 D61:D71 D13:D23 D10:D11 D48:D56">
-    <cfRule type="cellIs" dxfId="399" priority="85" operator="equal">
+    <cfRule type="cellIs" dxfId="407" priority="85" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="398" priority="86" operator="equal">
+    <cfRule type="cellIs" dxfId="406" priority="86" operator="equal">
       <formula>"Normal"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="397" priority="87" operator="equal">
+    <cfRule type="cellIs" dxfId="405" priority="87" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H91:H95">
-    <cfRule type="cellIs" dxfId="396" priority="81" operator="equal">
+    <cfRule type="cellIs" dxfId="404" priority="81" operator="equal">
       <formula>"Due/Overdue"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="395" priority="82" operator="equal">
+    <cfRule type="cellIs" dxfId="403" priority="82" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="394" priority="83" operator="equal">
+    <cfRule type="cellIs" dxfId="402" priority="83" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="393" priority="84" operator="equal">
+    <cfRule type="cellIs" dxfId="401" priority="84" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D91:D95">
-    <cfRule type="cellIs" dxfId="392" priority="78" operator="equal">
+    <cfRule type="cellIs" dxfId="400" priority="78" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="391" priority="79" operator="equal">
+    <cfRule type="cellIs" dxfId="399" priority="79" operator="equal">
       <formula>"Normal"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="390" priority="80" operator="equal">
+    <cfRule type="cellIs" dxfId="398" priority="80" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4:D9">
-    <cfRule type="cellIs" dxfId="389" priority="75" operator="equal">
+    <cfRule type="cellIs" dxfId="397" priority="75" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="388" priority="76" operator="equal">
+    <cfRule type="cellIs" dxfId="396" priority="76" operator="equal">
       <formula>"Normal"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="387" priority="77" operator="equal">
+    <cfRule type="cellIs" dxfId="395" priority="77" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4:H8">
-    <cfRule type="cellIs" dxfId="386" priority="71" operator="equal">
+    <cfRule type="cellIs" dxfId="394" priority="71" operator="equal">
       <formula>"Due/Overdue"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="385" priority="72" operator="equal">
+    <cfRule type="cellIs" dxfId="393" priority="72" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="384" priority="73" operator="equal">
+    <cfRule type="cellIs" dxfId="392" priority="73" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="383" priority="74" operator="equal">
+    <cfRule type="cellIs" dxfId="391" priority="74" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H9">
-    <cfRule type="cellIs" dxfId="382" priority="67" operator="equal">
+    <cfRule type="cellIs" dxfId="390" priority="67" operator="equal">
       <formula>"Due/Overdue"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="381" priority="68" operator="equal">
+    <cfRule type="cellIs" dxfId="389" priority="68" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="380" priority="69" operator="equal">
+    <cfRule type="cellIs" dxfId="388" priority="69" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="379" priority="70" operator="equal">
+    <cfRule type="cellIs" dxfId="387" priority="70" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H24">
-    <cfRule type="cellIs" dxfId="378" priority="63" operator="equal">
+    <cfRule type="cellIs" dxfId="386" priority="63" operator="equal">
       <formula>"Due/Overdue"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="377" priority="64" operator="equal">
+    <cfRule type="cellIs" dxfId="385" priority="64" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="376" priority="65" operator="equal">
+    <cfRule type="cellIs" dxfId="384" priority="65" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="375" priority="66" operator="equal">
+    <cfRule type="cellIs" dxfId="383" priority="66" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D24">
-    <cfRule type="cellIs" dxfId="374" priority="60" operator="equal">
+    <cfRule type="cellIs" dxfId="382" priority="60" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="373" priority="61" operator="equal">
+    <cfRule type="cellIs" dxfId="381" priority="61" operator="equal">
       <formula>"Normal"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="372" priority="62" operator="equal">
+    <cfRule type="cellIs" dxfId="380" priority="62" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H44:H45">
-    <cfRule type="cellIs" dxfId="371" priority="56" operator="equal">
+    <cfRule type="cellIs" dxfId="379" priority="56" operator="equal">
       <formula>"Due/Overdue"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="370" priority="57" operator="equal">
+    <cfRule type="cellIs" dxfId="378" priority="57" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="369" priority="58" operator="equal">
+    <cfRule type="cellIs" dxfId="377" priority="58" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="368" priority="59" operator="equal">
+    <cfRule type="cellIs" dxfId="376" priority="59" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D44:D45">
-    <cfRule type="cellIs" dxfId="367" priority="53" operator="equal">
+    <cfRule type="cellIs" dxfId="375" priority="53" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="366" priority="54" operator="equal">
+    <cfRule type="cellIs" dxfId="374" priority="54" operator="equal">
       <formula>"Normal"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="365" priority="55" operator="equal">
+    <cfRule type="cellIs" dxfId="373" priority="55" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H29">
-    <cfRule type="cellIs" dxfId="364" priority="49" operator="equal">
+    <cfRule type="cellIs" dxfId="372" priority="49" operator="equal">
       <formula>"Due/Overdue"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="363" priority="50" operator="equal">
+    <cfRule type="cellIs" dxfId="371" priority="50" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="362" priority="51" operator="equal">
+    <cfRule type="cellIs" dxfId="370" priority="51" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="361" priority="52" operator="equal">
+    <cfRule type="cellIs" dxfId="369" priority="52" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D29">
-    <cfRule type="cellIs" dxfId="360" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="368" priority="46" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="359" priority="47" operator="equal">
+    <cfRule type="cellIs" dxfId="367" priority="47" operator="equal">
       <formula>"Normal"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="358" priority="48" operator="equal">
+    <cfRule type="cellIs" dxfId="366" priority="48" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H76:H77">
-    <cfRule type="cellIs" dxfId="357" priority="42" operator="equal">
+    <cfRule type="cellIs" dxfId="365" priority="42" operator="equal">
       <formula>"Due/Overdue"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="356" priority="43" operator="equal">
+    <cfRule type="cellIs" dxfId="364" priority="43" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="355" priority="44" operator="equal">
+    <cfRule type="cellIs" dxfId="363" priority="44" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="354" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="362" priority="45" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D72 D76:D77">
-    <cfRule type="cellIs" dxfId="353" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="361" priority="39" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="352" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="360" priority="40" operator="equal">
       <formula>"Normal"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="351" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="359" priority="41" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D46:D47">
-    <cfRule type="cellIs" dxfId="350" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="358" priority="36" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="349" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="357" priority="37" operator="equal">
       <formula>"Normal"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="348" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="356" priority="38" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H46:H47">
-    <cfRule type="cellIs" dxfId="347" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="355" priority="32" operator="equal">
       <formula>"Due/Overdue"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="346" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="354" priority="33" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="345" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="353" priority="34" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="344" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="352" priority="35" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D12">
-    <cfRule type="cellIs" dxfId="343" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="351" priority="29" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="342" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="350" priority="30" operator="equal">
       <formula>"Normal"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="341" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="349" priority="31" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H12">
-    <cfRule type="cellIs" dxfId="340" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="348" priority="25" operator="equal">
       <formula>"Due/Overdue"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="339" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="347" priority="26" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="338" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="346" priority="27" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="337" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="345" priority="28" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D74:D75">
-    <cfRule type="cellIs" dxfId="336" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="344" priority="22" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="335" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="343" priority="23" operator="equal">
       <formula>"Normal"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="334" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="342" priority="24" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H74:H75">
-    <cfRule type="cellIs" dxfId="333" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="341" priority="19" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="332" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="340" priority="20" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="331" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="339" priority="21" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H72">
-    <cfRule type="cellIs" dxfId="330" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="338" priority="14" operator="equal">
       <formula>"Due/Overdue"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="329" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="337" priority="15" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="328" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="336" priority="16" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="327" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="335" priority="17" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H70:H75">
-    <cfRule type="cellIs" dxfId="326" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="334" priority="18" operator="equal">
       <formula>"Due/Overdue"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D57:D59">
-    <cfRule type="cellIs" dxfId="325" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="333" priority="8" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="324" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="332" priority="9" operator="equal">
       <formula>"Normal"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="323" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="331" priority="10" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D60">
-    <cfRule type="cellIs" dxfId="322" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="330" priority="5" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="321" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="329" priority="6" operator="equal">
       <formula>"Normal"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="320" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="328" priority="7" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H57:H59">
-    <cfRule type="cellIs" dxfId="319" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="327" priority="1" operator="equal">
       <formula>"Due/Overdue"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="318" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="326" priority="2" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="317" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="325" priority="3" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="316" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="324" priority="4" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H1 H4:H41 H43:H59 H61:H1048576" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H1 H4:H41 H43:H59 H61:H1048576">
       <formula1>"Pending, In Progress, Done,Due/Overdue"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D41 D43:D1048576" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D41 D43:D1048576">
       <formula1>"Low,Normal,High"</formula1>
     </dataValidation>
   </dataValidations>
@@ -8876,23 +8944,23 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:I63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0" xr3:uid="{958C4451-9541-5A59-BF78-D2F731DF1C81}">
-      <selection activeCell="I25" sqref="I25"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="I45" sqref="I45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" customWidth="1"/>
-    <col min="3" max="3" width="35.42578125" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" style="51"/>
+    <col min="1" max="1" width="2.6640625" customWidth="1"/>
+    <col min="3" max="3" width="35.44140625" customWidth="1"/>
+    <col min="6" max="6" width="11.44140625" style="51"/>
     <col min="7" max="7" width="14" customWidth="1"/>
-    <col min="9" max="9" width="32.28515625" customWidth="1"/>
+    <col min="9" max="9" width="32.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" ht="31.5">
+    <row r="2" spans="2:9" ht="31.2" x14ac:dyDescent="0.3">
       <c r="B2" s="10" t="s">
         <v>167</v>
       </c>
@@ -8904,7 +8972,7 @@
       <c r="H2" s="31"/>
       <c r="I2" s="32"/>
     </row>
-    <row r="3" spans="2:9" ht="31.5">
+    <row r="3" spans="2:9" ht="31.2" x14ac:dyDescent="0.3">
       <c r="B3" s="44" t="s">
         <v>2</v>
       </c>
@@ -8930,7 +8998,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="2:9" ht="64.5" customHeight="1">
+    <row r="4" spans="2:9" ht="64.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="84" t="s">
         <v>10</v>
       </c>
@@ -8954,7 +9022,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="5" spans="2:9" ht="26.25">
+    <row r="5" spans="2:9" ht="27.6" x14ac:dyDescent="0.3">
       <c r="B5" s="85"/>
       <c r="C5" s="40" t="s">
         <v>170</v>
@@ -8976,7 +9044,7 @@
       </c>
       <c r="I5" s="26"/>
     </row>
-    <row r="6" spans="2:9" ht="30">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B6" s="85"/>
       <c r="C6" s="26" t="s">
         <v>172</v>
@@ -9000,7 +9068,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="7" spans="2:9">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B7" s="85"/>
       <c r="C7" s="26" t="s">
         <v>174</v>
@@ -9022,7 +9090,7 @@
       </c>
       <c r="I7" s="26"/>
     </row>
-    <row r="8" spans="2:9">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B8" s="85"/>
       <c r="C8" s="26" t="s">
         <v>175</v>
@@ -9044,7 +9112,7 @@
       </c>
       <c r="I8" s="26"/>
     </row>
-    <row r="9" spans="2:9">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B9" s="85"/>
       <c r="C9" s="53" t="s">
         <v>177</v>
@@ -9066,7 +9134,7 @@
       </c>
       <c r="I9" s="53"/>
     </row>
-    <row r="10" spans="2:9">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B10" s="86"/>
       <c r="C10" s="38"/>
       <c r="D10" s="13"/>
@@ -9076,7 +9144,7 @@
       <c r="H10" s="17"/>
       <c r="I10" s="28"/>
     </row>
-    <row r="11" spans="2:9" ht="25.5">
+    <row r="11" spans="2:9" ht="27.6" x14ac:dyDescent="0.3">
       <c r="B11" s="84" t="s">
         <v>179</v>
       </c>
@@ -9102,7 +9170,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="12" spans="2:9">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B12" s="85"/>
       <c r="C12" s="26" t="s">
         <v>184</v>
@@ -9124,7 +9192,7 @@
       </c>
       <c r="I12" s="26"/>
     </row>
-    <row r="13" spans="2:9">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B13" s="85"/>
       <c r="C13" s="26" t="s">
         <v>185</v>
@@ -9146,7 +9214,7 @@
       </c>
       <c r="I13" s="26"/>
     </row>
-    <row r="14" spans="2:9" ht="25.5">
+    <row r="14" spans="2:9" ht="27.6" x14ac:dyDescent="0.3">
       <c r="B14" s="85"/>
       <c r="C14" s="26" t="s">
         <v>186</v>
@@ -9168,7 +9236,7 @@
       </c>
       <c r="I14" s="26"/>
     </row>
-    <row r="15" spans="2:9">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B15" s="85"/>
       <c r="C15" s="26" t="s">
         <v>188</v>
@@ -9190,7 +9258,7 @@
       </c>
       <c r="I15" s="26"/>
     </row>
-    <row r="16" spans="2:9">
+    <row r="16" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B16" s="85"/>
       <c r="C16" s="53" t="s">
         <v>189</v>
@@ -9212,7 +9280,7 @@
       </c>
       <c r="I16" s="53"/>
     </row>
-    <row r="17" spans="2:9">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B17" s="85"/>
       <c r="C17" s="53" t="s">
         <v>190</v>
@@ -9234,7 +9302,7 @@
       </c>
       <c r="I17" s="53"/>
     </row>
-    <row r="18" spans="2:9" ht="25.5">
+    <row r="18" spans="2:9" ht="27.6" x14ac:dyDescent="0.3">
       <c r="B18" s="85"/>
       <c r="C18" s="53" t="s">
         <v>191</v>
@@ -9258,7 +9326,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="19" spans="2:9">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B19" s="85"/>
       <c r="C19" s="53" t="s">
         <v>193</v>
@@ -9280,7 +9348,7 @@
       </c>
       <c r="I19" s="53"/>
     </row>
-    <row r="20" spans="2:9">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B20" s="86"/>
       <c r="C20" s="38"/>
       <c r="D20" s="13"/>
@@ -9290,7 +9358,7 @@
       <c r="H20" s="17"/>
       <c r="I20" s="28"/>
     </row>
-    <row r="21" spans="2:9" ht="14.25">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B21" s="89" t="s">
         <v>194</v>
       </c>
@@ -9316,7 +9384,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="22" spans="2:9">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B22" s="85"/>
       <c r="C22" s="26" t="s">
         <v>184</v>
@@ -9338,7 +9406,7 @@
       </c>
       <c r="I22" s="26"/>
     </row>
-    <row r="23" spans="2:9" ht="45">
+    <row r="23" spans="2:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B23" s="85"/>
       <c r="C23" s="26" t="s">
         <v>197</v>
@@ -9362,7 +9430,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="24" spans="2:9" ht="51">
+    <row r="24" spans="2:9" ht="55.2" x14ac:dyDescent="0.3">
       <c r="B24" s="85"/>
       <c r="C24" s="26" t="s">
         <v>200</v>
@@ -9386,7 +9454,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="25" spans="2:9">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B25" s="85"/>
       <c r="C25" s="26" t="s">
         <v>202</v>
@@ -9408,7 +9476,7 @@
       </c>
       <c r="I25" s="26"/>
     </row>
-    <row r="26" spans="2:9">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B26" s="85"/>
       <c r="C26" s="53" t="s">
         <v>203</v>
@@ -9430,7 +9498,7 @@
       </c>
       <c r="I26" s="53"/>
     </row>
-    <row r="27" spans="2:9">
+    <row r="27" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B27" s="85"/>
       <c r="C27" s="53" t="s">
         <v>204</v>
@@ -9452,7 +9520,7 @@
       </c>
       <c r="I27" s="53"/>
     </row>
-    <row r="28" spans="2:9">
+    <row r="28" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B28" s="86"/>
       <c r="C28" s="38"/>
       <c r="D28" s="13"/>
@@ -9462,7 +9530,7 @@
       <c r="H28" s="17"/>
       <c r="I28" s="28"/>
     </row>
-    <row r="29" spans="2:9">
+    <row r="29" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B29" s="89" t="s">
         <v>205</v>
       </c>
@@ -9488,7 +9556,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="30" spans="2:9" ht="38.25">
+    <row r="30" spans="2:9" ht="41.4" x14ac:dyDescent="0.3">
       <c r="B30" s="85"/>
       <c r="C30" s="26" t="s">
         <v>184</v>
@@ -9512,7 +9580,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="31" spans="2:9">
+    <row r="31" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B31" s="85"/>
       <c r="C31" s="26" t="s">
         <v>209</v>
@@ -9534,7 +9602,7 @@
       </c>
       <c r="I31" s="26"/>
     </row>
-    <row r="32" spans="2:9" ht="25.5">
+    <row r="32" spans="2:9" ht="27.6" x14ac:dyDescent="0.3">
       <c r="B32" s="85"/>
       <c r="C32" s="26" t="s">
         <v>210</v>
@@ -9556,7 +9624,7 @@
       </c>
       <c r="I32" s="26"/>
     </row>
-    <row r="33" spans="2:9">
+    <row r="33" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B33" s="85"/>
       <c r="C33" s="26" t="s">
         <v>211</v>
@@ -9578,7 +9646,7 @@
       </c>
       <c r="I33" s="26"/>
     </row>
-    <row r="34" spans="2:9">
+    <row r="34" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B34" s="85"/>
       <c r="C34" s="26" t="s">
         <v>212</v>
@@ -9600,7 +9668,7 @@
       </c>
       <c r="I34" s="53"/>
     </row>
-    <row r="35" spans="2:9">
+    <row r="35" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B35" s="86"/>
       <c r="C35" s="38"/>
       <c r="D35" s="13"/>
@@ -9610,7 +9678,7 @@
       <c r="H35" s="17"/>
       <c r="I35" s="28"/>
     </row>
-    <row r="36" spans="2:9" ht="14.25">
+    <row r="36" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B36" s="84" t="s">
         <v>213</v>
       </c>
@@ -9636,7 +9704,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="37" spans="2:9">
+    <row r="37" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B37" s="85"/>
       <c r="C37" s="26" t="s">
         <v>184</v>
@@ -9658,7 +9726,7 @@
       </c>
       <c r="I37" s="26"/>
     </row>
-    <row r="38" spans="2:9">
+    <row r="38" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B38" s="85"/>
       <c r="C38" s="26" t="s">
         <v>215</v>
@@ -9680,7 +9748,7 @@
       </c>
       <c r="I38" s="26"/>
     </row>
-    <row r="39" spans="2:9">
+    <row r="39" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B39" s="85"/>
       <c r="C39" s="26" t="s">
         <v>216</v>
@@ -9702,7 +9770,7 @@
       </c>
       <c r="I39" s="26"/>
     </row>
-    <row r="40" spans="2:9">
+    <row r="40" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B40" s="85"/>
       <c r="C40" s="26"/>
       <c r="D40" s="11"/>
@@ -9712,7 +9780,7 @@
       <c r="H40" s="12"/>
       <c r="I40" s="26"/>
     </row>
-    <row r="41" spans="2:9">
+    <row r="41" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B41" s="86"/>
       <c r="C41" s="38"/>
       <c r="D41" s="13"/>
@@ -9722,7 +9790,7 @@
       <c r="H41" s="17"/>
       <c r="I41" s="28"/>
     </row>
-    <row r="42" spans="2:9" ht="15" customHeight="1">
+    <row r="42" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B42" s="84" t="s">
         <v>217</v>
       </c>
@@ -9748,7 +9816,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="43" spans="2:9">
+    <row r="43" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B43" s="85"/>
       <c r="C43" s="26" t="s">
         <v>184</v>
@@ -9770,7 +9838,7 @@
       </c>
       <c r="I43" s="26"/>
     </row>
-    <row r="44" spans="2:9" ht="25.5">
+    <row r="44" spans="2:9" ht="27.6" x14ac:dyDescent="0.3">
       <c r="B44" s="85"/>
       <c r="C44" s="26" t="s">
         <v>220</v>
@@ -9790,9 +9858,11 @@
       <c r="H44" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="I44" s="26"/>
-    </row>
-    <row r="45" spans="2:9">
+      <c r="I44" s="26" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="45" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B45" s="85"/>
       <c r="C45" s="26" t="s">
         <v>221</v>
@@ -9810,11 +9880,11 @@
         <v>218</v>
       </c>
       <c r="H45" s="16" t="s">
-        <v>65</v>
+        <v>15</v>
       </c>
       <c r="I45" s="26"/>
     </row>
-    <row r="46" spans="2:9">
+    <row r="46" spans="2:9" ht="27.6" x14ac:dyDescent="0.3">
       <c r="B46" s="85"/>
       <c r="C46" s="26" t="s">
         <v>222</v>
@@ -9831,12 +9901,14 @@
       <c r="G46" s="26" t="s">
         <v>218</v>
       </c>
-      <c r="H46" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="I46" s="26"/>
-    </row>
-    <row r="47" spans="2:9" ht="25.5">
+      <c r="H46" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="I46" s="26" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="47" spans="2:9" ht="27.6" x14ac:dyDescent="0.3">
       <c r="B47" s="85"/>
       <c r="C47" s="26" t="s">
         <v>223</v>
@@ -9854,11 +9926,13 @@
         <v>218</v>
       </c>
       <c r="H47" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="I47" s="53"/>
-    </row>
-    <row r="48" spans="2:9">
+        <v>15</v>
+      </c>
+      <c r="I47" s="53" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="48" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B48" s="86"/>
       <c r="C48" s="38"/>
       <c r="D48" s="13"/>
@@ -9868,7 +9942,7 @@
       <c r="H48" s="17"/>
       <c r="I48" s="28"/>
     </row>
-    <row r="49" spans="2:9" ht="30" customHeight="1">
+    <row r="49" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B49" s="84" t="s">
         <v>224</v>
       </c>
@@ -9890,7 +9964,7 @@
       </c>
       <c r="I49" s="26"/>
     </row>
-    <row r="50" spans="2:9">
+    <row r="50" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B50" s="85"/>
       <c r="C50" s="26" t="s">
         <v>180</v>
@@ -9914,7 +9988,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="51" spans="2:9">
+    <row r="51" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B51" s="85"/>
       <c r="C51" s="26" t="s">
         <v>184</v>
@@ -9936,7 +10010,7 @@
       </c>
       <c r="I51" s="26"/>
     </row>
-    <row r="52" spans="2:9">
+    <row r="52" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B52" s="85"/>
       <c r="C52" s="26" t="s">
         <v>228</v>
@@ -9958,7 +10032,7 @@
       </c>
       <c r="I52" s="26"/>
     </row>
-    <row r="53" spans="2:9">
+    <row r="53" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B53" s="85"/>
       <c r="C53" s="26" t="s">
         <v>229</v>
@@ -9980,7 +10054,7 @@
       </c>
       <c r="I53" s="26"/>
     </row>
-    <row r="54" spans="2:9">
+    <row r="54" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B54" s="85"/>
       <c r="C54" s="26" t="s">
         <v>230</v>
@@ -10002,7 +10076,7 @@
       </c>
       <c r="I54" s="53"/>
     </row>
-    <row r="55" spans="2:9">
+    <row r="55" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B55" s="86"/>
       <c r="C55" s="38"/>
       <c r="D55" s="13"/>
@@ -10012,7 +10086,7 @@
       <c r="H55" s="17"/>
       <c r="I55" s="28"/>
     </row>
-    <row r="56" spans="2:9">
+    <row r="56" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B56" s="84" t="s">
         <v>231</v>
       </c>
@@ -10038,7 +10112,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="57" spans="2:9">
+    <row r="57" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B57" s="85"/>
       <c r="C57" s="26" t="s">
         <v>184</v>
@@ -10060,7 +10134,7 @@
       </c>
       <c r="I57" s="26"/>
     </row>
-    <row r="58" spans="2:9">
+    <row r="58" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B58" s="85"/>
       <c r="C58" s="26" t="s">
         <v>234</v>
@@ -10082,7 +10156,7 @@
       </c>
       <c r="I58" s="26"/>
     </row>
-    <row r="59" spans="2:9">
+    <row r="59" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B59" s="85"/>
       <c r="C59" s="26" t="s">
         <v>209</v>
@@ -10104,7 +10178,7 @@
       </c>
       <c r="I59" s="26"/>
     </row>
-    <row r="60" spans="2:9">
+    <row r="60" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B60" s="85"/>
       <c r="C60" s="26" t="s">
         <v>236</v>
@@ -10126,7 +10200,7 @@
       </c>
       <c r="I60" s="26"/>
     </row>
-    <row r="61" spans="2:9">
+    <row r="61" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B61" s="85"/>
       <c r="C61" s="26" t="s">
         <v>211</v>
@@ -10148,7 +10222,7 @@
       </c>
       <c r="I61" s="26"/>
     </row>
-    <row r="62" spans="2:9">
+    <row r="62" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B62" s="85"/>
       <c r="C62" s="26" t="s">
         <v>212</v>
@@ -10170,7 +10244,7 @@
       </c>
       <c r="I62" s="53"/>
     </row>
-    <row r="63" spans="2:9">
+    <row r="63" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B63" s="86"/>
       <c r="C63" s="38"/>
       <c r="D63" s="13"/>
@@ -10181,7 +10255,7 @@
       <c r="I63" s="28"/>
     </row>
   </sheetData>
-  <autoFilter ref="B3:I3" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
+  <autoFilter ref="B3:I3"/>
   <mergeCells count="8">
     <mergeCell ref="B56:B63"/>
     <mergeCell ref="B4:B10"/>
@@ -10193,1162 +10267,1171 @@
     <mergeCell ref="B42:B48"/>
   </mergeCells>
   <conditionalFormatting sqref="H40 H4 H23 H25">
-    <cfRule type="cellIs" dxfId="315" priority="418" operator="equal">
+    <cfRule type="cellIs" dxfId="323" priority="422" operator="equal">
       <formula>"Due/Overdue"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="314" priority="419" operator="equal">
+    <cfRule type="cellIs" dxfId="322" priority="423" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="313" priority="420" operator="equal">
+    <cfRule type="cellIs" dxfId="321" priority="424" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="312" priority="421" operator="equal">
+    <cfRule type="cellIs" dxfId="320" priority="425" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D40:D41 D2:D4 D23 D25:D28">
-    <cfRule type="cellIs" dxfId="311" priority="415" operator="equal">
+    <cfRule type="cellIs" dxfId="319" priority="419" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="310" priority="416" operator="equal">
+    <cfRule type="cellIs" dxfId="318" priority="420" operator="equal">
       <formula>"Normal"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="309" priority="417" operator="equal">
+    <cfRule type="cellIs" dxfId="317" priority="421" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H41">
-    <cfRule type="cellIs" dxfId="308" priority="349" operator="equal">
+    <cfRule type="cellIs" dxfId="316" priority="353" operator="equal">
       <formula>"Due/Overdue"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="307" priority="350" operator="equal">
+    <cfRule type="cellIs" dxfId="315" priority="354" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="306" priority="351" operator="equal">
+    <cfRule type="cellIs" dxfId="314" priority="355" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="305" priority="352" operator="equal">
+    <cfRule type="cellIs" dxfId="313" priority="356" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D49 D52 D55">
-    <cfRule type="cellIs" dxfId="304" priority="346" operator="equal">
+    <cfRule type="cellIs" dxfId="312" priority="350" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="303" priority="347" operator="equal">
+    <cfRule type="cellIs" dxfId="311" priority="351" operator="equal">
       <formula>"Normal"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="302" priority="348" operator="equal">
+    <cfRule type="cellIs" dxfId="310" priority="352" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H49">
-    <cfRule type="cellIs" dxfId="301" priority="342" operator="equal">
+    <cfRule type="cellIs" dxfId="309" priority="346" operator="equal">
       <formula>"Due/Overdue"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="300" priority="343" operator="equal">
+    <cfRule type="cellIs" dxfId="308" priority="347" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="299" priority="344" operator="equal">
+    <cfRule type="cellIs" dxfId="307" priority="348" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="298" priority="345" operator="equal">
+    <cfRule type="cellIs" dxfId="306" priority="349" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H55">
-    <cfRule type="cellIs" dxfId="297" priority="338" operator="equal">
+    <cfRule type="cellIs" dxfId="305" priority="342" operator="equal">
       <formula>"Due/Overdue"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="296" priority="339" operator="equal">
+    <cfRule type="cellIs" dxfId="304" priority="343" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="295" priority="340" operator="equal">
+    <cfRule type="cellIs" dxfId="303" priority="344" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="294" priority="341" operator="equal">
+    <cfRule type="cellIs" dxfId="302" priority="345" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D11:D15 D20">
-    <cfRule type="cellIs" dxfId="293" priority="335" operator="equal">
+    <cfRule type="cellIs" dxfId="301" priority="339" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="292" priority="336" operator="equal">
+    <cfRule type="cellIs" dxfId="300" priority="340" operator="equal">
       <formula>"Normal"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="291" priority="337" operator="equal">
+    <cfRule type="cellIs" dxfId="299" priority="341" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H11:H15">
-    <cfRule type="cellIs" dxfId="290" priority="331" operator="equal">
+    <cfRule type="cellIs" dxfId="298" priority="335" operator="equal">
       <formula>"Due/Overdue"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="289" priority="332" operator="equal">
+    <cfRule type="cellIs" dxfId="297" priority="336" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="288" priority="333" operator="equal">
+    <cfRule type="cellIs" dxfId="296" priority="337" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="287" priority="334" operator="equal">
+    <cfRule type="cellIs" dxfId="295" priority="338" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H20">
-    <cfRule type="cellIs" dxfId="286" priority="327" operator="equal">
+    <cfRule type="cellIs" dxfId="294" priority="331" operator="equal">
       <formula>"Due/Overdue"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="285" priority="328" operator="equal">
+    <cfRule type="cellIs" dxfId="293" priority="332" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="284" priority="329" operator="equal">
+    <cfRule type="cellIs" dxfId="292" priority="333" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="283" priority="330" operator="equal">
+    <cfRule type="cellIs" dxfId="291" priority="334" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H28">
-    <cfRule type="cellIs" dxfId="282" priority="316" operator="equal">
+    <cfRule type="cellIs" dxfId="290" priority="320" operator="equal">
       <formula>"Due/Overdue"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="281" priority="317" operator="equal">
+    <cfRule type="cellIs" dxfId="289" priority="321" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="280" priority="318" operator="equal">
+    <cfRule type="cellIs" dxfId="288" priority="322" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="279" priority="319" operator="equal">
+    <cfRule type="cellIs" dxfId="287" priority="323" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D31 D35">
-    <cfRule type="cellIs" dxfId="278" priority="313" operator="equal">
+    <cfRule type="cellIs" dxfId="286" priority="317" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="277" priority="314" operator="equal">
+    <cfRule type="cellIs" dxfId="285" priority="318" operator="equal">
       <formula>"Normal"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="276" priority="315" operator="equal">
+    <cfRule type="cellIs" dxfId="284" priority="319" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H31">
-    <cfRule type="cellIs" dxfId="275" priority="309" operator="equal">
+    <cfRule type="cellIs" dxfId="283" priority="313" operator="equal">
       <formula>"Due/Overdue"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="274" priority="310" operator="equal">
+    <cfRule type="cellIs" dxfId="282" priority="314" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="273" priority="311" operator="equal">
+    <cfRule type="cellIs" dxfId="281" priority="315" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="272" priority="312" operator="equal">
+    <cfRule type="cellIs" dxfId="280" priority="316" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H35">
-    <cfRule type="cellIs" dxfId="271" priority="305" operator="equal">
+    <cfRule type="cellIs" dxfId="279" priority="309" operator="equal">
       <formula>"Due/Overdue"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="270" priority="306" operator="equal">
+    <cfRule type="cellIs" dxfId="278" priority="310" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="269" priority="307" operator="equal">
+    <cfRule type="cellIs" dxfId="277" priority="311" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="268" priority="308" operator="equal">
+    <cfRule type="cellIs" dxfId="276" priority="312" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6:D10">
-    <cfRule type="cellIs" dxfId="267" priority="302" operator="equal">
+    <cfRule type="cellIs" dxfId="275" priority="306" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="266" priority="303" operator="equal">
+    <cfRule type="cellIs" dxfId="274" priority="307" operator="equal">
       <formula>"Normal"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="265" priority="304" operator="equal">
+    <cfRule type="cellIs" dxfId="273" priority="308" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H6:H9">
-    <cfRule type="cellIs" dxfId="264" priority="298" operator="equal">
+    <cfRule type="cellIs" dxfId="272" priority="302" operator="equal">
       <formula>"Due/Overdue"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="263" priority="299" operator="equal">
+    <cfRule type="cellIs" dxfId="271" priority="303" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="262" priority="300" operator="equal">
+    <cfRule type="cellIs" dxfId="270" priority="304" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="261" priority="301" operator="equal">
+    <cfRule type="cellIs" dxfId="269" priority="305" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H10">
-    <cfRule type="cellIs" dxfId="260" priority="294" operator="equal">
+    <cfRule type="cellIs" dxfId="268" priority="298" operator="equal">
       <formula>"Due/Overdue"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="259" priority="295" operator="equal">
+    <cfRule type="cellIs" dxfId="267" priority="299" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="258" priority="296" operator="equal">
+    <cfRule type="cellIs" dxfId="266" priority="300" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="257" priority="297" operator="equal">
+    <cfRule type="cellIs" dxfId="265" priority="301" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5">
-    <cfRule type="cellIs" dxfId="256" priority="291" operator="equal">
+    <cfRule type="cellIs" dxfId="264" priority="295" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="255" priority="292" operator="equal">
+    <cfRule type="cellIs" dxfId="263" priority="296" operator="equal">
       <formula>"Normal"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="254" priority="293" operator="equal">
+    <cfRule type="cellIs" dxfId="262" priority="297" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5">
-    <cfRule type="cellIs" dxfId="253" priority="287" operator="equal">
+    <cfRule type="cellIs" dxfId="261" priority="291" operator="equal">
       <formula>"Due/Overdue"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="252" priority="288" operator="equal">
+    <cfRule type="cellIs" dxfId="260" priority="292" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="251" priority="289" operator="equal">
+    <cfRule type="cellIs" dxfId="259" priority="293" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="250" priority="290" operator="equal">
+    <cfRule type="cellIs" dxfId="258" priority="294" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D21">
-    <cfRule type="cellIs" dxfId="249" priority="284" operator="equal">
+    <cfRule type="cellIs" dxfId="257" priority="288" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="248" priority="285" operator="equal">
+    <cfRule type="cellIs" dxfId="256" priority="289" operator="equal">
       <formula>"Normal"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="247" priority="286" operator="equal">
+    <cfRule type="cellIs" dxfId="255" priority="290" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H21">
-    <cfRule type="cellIs" dxfId="246" priority="280" operator="equal">
+    <cfRule type="cellIs" dxfId="254" priority="284" operator="equal">
       <formula>"Due/Overdue"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="245" priority="281" operator="equal">
+    <cfRule type="cellIs" dxfId="253" priority="285" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="244" priority="282" operator="equal">
+    <cfRule type="cellIs" dxfId="252" priority="286" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="243" priority="283" operator="equal">
+    <cfRule type="cellIs" dxfId="251" priority="287" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D29">
-    <cfRule type="cellIs" dxfId="242" priority="277" operator="equal">
+    <cfRule type="cellIs" dxfId="250" priority="281" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="241" priority="278" operator="equal">
+    <cfRule type="cellIs" dxfId="249" priority="282" operator="equal">
       <formula>"Normal"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="240" priority="279" operator="equal">
+    <cfRule type="cellIs" dxfId="248" priority="283" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H29">
-    <cfRule type="cellIs" dxfId="239" priority="273" operator="equal">
+    <cfRule type="cellIs" dxfId="247" priority="277" operator="equal">
       <formula>"Due/Overdue"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="238" priority="274" operator="equal">
+    <cfRule type="cellIs" dxfId="246" priority="278" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="237" priority="275" operator="equal">
+    <cfRule type="cellIs" dxfId="245" priority="279" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="236" priority="276" operator="equal">
+    <cfRule type="cellIs" dxfId="244" priority="280" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D36">
-    <cfRule type="cellIs" dxfId="235" priority="270" operator="equal">
+    <cfRule type="cellIs" dxfId="243" priority="274" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="234" priority="271" operator="equal">
+    <cfRule type="cellIs" dxfId="242" priority="275" operator="equal">
       <formula>"Normal"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="233" priority="272" operator="equal">
+    <cfRule type="cellIs" dxfId="241" priority="276" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H36">
-    <cfRule type="cellIs" dxfId="232" priority="266" operator="equal">
+    <cfRule type="cellIs" dxfId="240" priority="270" operator="equal">
       <formula>"Due/Overdue"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="231" priority="267" operator="equal">
+    <cfRule type="cellIs" dxfId="239" priority="271" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="230" priority="268" operator="equal">
+    <cfRule type="cellIs" dxfId="238" priority="272" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="229" priority="269" operator="equal">
+    <cfRule type="cellIs" dxfId="237" priority="273" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D50">
-    <cfRule type="cellIs" dxfId="228" priority="263" operator="equal">
+    <cfRule type="cellIs" dxfId="236" priority="267" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="227" priority="264" operator="equal">
+    <cfRule type="cellIs" dxfId="235" priority="268" operator="equal">
       <formula>"Normal"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="226" priority="265" operator="equal">
+    <cfRule type="cellIs" dxfId="234" priority="269" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H50">
-    <cfRule type="cellIs" dxfId="225" priority="259" operator="equal">
+    <cfRule type="cellIs" dxfId="233" priority="263" operator="equal">
       <formula>"Due/Overdue"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="224" priority="260" operator="equal">
+    <cfRule type="cellIs" dxfId="232" priority="264" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="223" priority="261" operator="equal">
+    <cfRule type="cellIs" dxfId="231" priority="265" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="222" priority="262" operator="equal">
+    <cfRule type="cellIs" dxfId="230" priority="266" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D22">
-    <cfRule type="cellIs" dxfId="221" priority="256" operator="equal">
+    <cfRule type="cellIs" dxfId="229" priority="260" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="220" priority="257" operator="equal">
+    <cfRule type="cellIs" dxfId="228" priority="261" operator="equal">
       <formula>"Normal"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="219" priority="258" operator="equal">
+    <cfRule type="cellIs" dxfId="227" priority="262" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H22">
-    <cfRule type="cellIs" dxfId="218" priority="252" operator="equal">
+    <cfRule type="cellIs" dxfId="226" priority="256" operator="equal">
       <formula>"Due/Overdue"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="217" priority="253" operator="equal">
+    <cfRule type="cellIs" dxfId="225" priority="257" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="216" priority="254" operator="equal">
+    <cfRule type="cellIs" dxfId="224" priority="258" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="215" priority="255" operator="equal">
+    <cfRule type="cellIs" dxfId="223" priority="259" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D30">
-    <cfRule type="cellIs" dxfId="214" priority="249" operator="equal">
+    <cfRule type="cellIs" dxfId="222" priority="253" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="213" priority="250" operator="equal">
+    <cfRule type="cellIs" dxfId="221" priority="254" operator="equal">
       <formula>"Normal"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="212" priority="251" operator="equal">
+    <cfRule type="cellIs" dxfId="220" priority="255" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H30">
-    <cfRule type="cellIs" dxfId="211" priority="245" operator="equal">
+    <cfRule type="cellIs" dxfId="219" priority="249" operator="equal">
       <formula>"Due/Overdue"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="210" priority="246" operator="equal">
+    <cfRule type="cellIs" dxfId="218" priority="250" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="209" priority="247" operator="equal">
+    <cfRule type="cellIs" dxfId="217" priority="251" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="208" priority="248" operator="equal">
+    <cfRule type="cellIs" dxfId="216" priority="252" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D37">
-    <cfRule type="cellIs" dxfId="207" priority="242" operator="equal">
+    <cfRule type="cellIs" dxfId="215" priority="246" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="206" priority="243" operator="equal">
+    <cfRule type="cellIs" dxfId="214" priority="247" operator="equal">
       <formula>"Normal"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="205" priority="244" operator="equal">
+    <cfRule type="cellIs" dxfId="213" priority="248" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H37">
-    <cfRule type="cellIs" dxfId="204" priority="238" operator="equal">
+    <cfRule type="cellIs" dxfId="212" priority="242" operator="equal">
       <formula>"Due/Overdue"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="203" priority="239" operator="equal">
+    <cfRule type="cellIs" dxfId="211" priority="243" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="202" priority="240" operator="equal">
+    <cfRule type="cellIs" dxfId="210" priority="244" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="201" priority="241" operator="equal">
+    <cfRule type="cellIs" dxfId="209" priority="245" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D51">
-    <cfRule type="cellIs" dxfId="200" priority="235" operator="equal">
+    <cfRule type="cellIs" dxfId="208" priority="239" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="199" priority="236" operator="equal">
+    <cfRule type="cellIs" dxfId="207" priority="240" operator="equal">
       <formula>"Normal"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="198" priority="237" operator="equal">
+    <cfRule type="cellIs" dxfId="206" priority="241" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H51">
-    <cfRule type="cellIs" dxfId="197" priority="231" operator="equal">
+    <cfRule type="cellIs" dxfId="205" priority="235" operator="equal">
       <formula>"Due/Overdue"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="196" priority="232" operator="equal">
+    <cfRule type="cellIs" dxfId="204" priority="236" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="195" priority="233" operator="equal">
+    <cfRule type="cellIs" dxfId="203" priority="237" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="194" priority="234" operator="equal">
+    <cfRule type="cellIs" dxfId="202" priority="238" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D38">
-    <cfRule type="cellIs" dxfId="193" priority="228" operator="equal">
+    <cfRule type="cellIs" dxfId="201" priority="232" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="192" priority="229" operator="equal">
+    <cfRule type="cellIs" dxfId="200" priority="233" operator="equal">
       <formula>"Normal"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="191" priority="230" operator="equal">
+    <cfRule type="cellIs" dxfId="199" priority="234" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H38">
-    <cfRule type="cellIs" dxfId="190" priority="224" operator="equal">
+    <cfRule type="cellIs" dxfId="198" priority="228" operator="equal">
       <formula>"Due/Overdue"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="189" priority="225" operator="equal">
+    <cfRule type="cellIs" dxfId="197" priority="229" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="188" priority="226" operator="equal">
+    <cfRule type="cellIs" dxfId="196" priority="230" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="187" priority="227" operator="equal">
+    <cfRule type="cellIs" dxfId="195" priority="231" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H48">
-    <cfRule type="cellIs" dxfId="186" priority="206" operator="equal">
+    <cfRule type="cellIs" dxfId="194" priority="210" operator="equal">
       <formula>"Due/Overdue"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="185" priority="207" operator="equal">
+    <cfRule type="cellIs" dxfId="193" priority="211" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="184" priority="208" operator="equal">
+    <cfRule type="cellIs" dxfId="192" priority="212" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="183" priority="209" operator="equal">
+    <cfRule type="cellIs" dxfId="191" priority="213" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D48">
-    <cfRule type="cellIs" dxfId="182" priority="210" operator="equal">
+    <cfRule type="cellIs" dxfId="190" priority="214" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="181" priority="211" operator="equal">
+    <cfRule type="cellIs" dxfId="189" priority="215" operator="equal">
       <formula>"Normal"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="180" priority="212" operator="equal">
+    <cfRule type="cellIs" dxfId="188" priority="216" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H57:H58">
-    <cfRule type="cellIs" dxfId="179" priority="153" operator="equal">
+    <cfRule type="cellIs" dxfId="187" priority="157" operator="equal">
       <formula>"Due/Overdue"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="178" priority="154" operator="equal">
+    <cfRule type="cellIs" dxfId="186" priority="158" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="177" priority="155" operator="equal">
+    <cfRule type="cellIs" dxfId="185" priority="159" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="176" priority="156" operator="equal">
+    <cfRule type="cellIs" dxfId="184" priority="160" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D42">
-    <cfRule type="cellIs" dxfId="175" priority="203" operator="equal">
+    <cfRule type="cellIs" dxfId="183" priority="207" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="174" priority="204" operator="equal">
+    <cfRule type="cellIs" dxfId="182" priority="208" operator="equal">
       <formula>"Normal"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="173" priority="205" operator="equal">
+    <cfRule type="cellIs" dxfId="181" priority="209" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H42">
-    <cfRule type="cellIs" dxfId="172" priority="199" operator="equal">
+    <cfRule type="cellIs" dxfId="180" priority="203" operator="equal">
       <formula>"Due/Overdue"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="171" priority="200" operator="equal">
+    <cfRule type="cellIs" dxfId="179" priority="204" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="170" priority="201" operator="equal">
+    <cfRule type="cellIs" dxfId="178" priority="205" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="169" priority="202" operator="equal">
+    <cfRule type="cellIs" dxfId="177" priority="206" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D43">
-    <cfRule type="cellIs" dxfId="168" priority="196" operator="equal">
+    <cfRule type="cellIs" dxfId="176" priority="200" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="167" priority="197" operator="equal">
+    <cfRule type="cellIs" dxfId="175" priority="201" operator="equal">
       <formula>"Normal"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="166" priority="198" operator="equal">
+    <cfRule type="cellIs" dxfId="174" priority="202" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H43">
-    <cfRule type="cellIs" dxfId="165" priority="192" operator="equal">
+    <cfRule type="cellIs" dxfId="173" priority="196" operator="equal">
       <formula>"Due/Overdue"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="164" priority="193" operator="equal">
+    <cfRule type="cellIs" dxfId="172" priority="197" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="163" priority="194" operator="equal">
+    <cfRule type="cellIs" dxfId="171" priority="198" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="162" priority="195" operator="equal">
+    <cfRule type="cellIs" dxfId="170" priority="199" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D44">
-    <cfRule type="cellIs" dxfId="161" priority="189" operator="equal">
+    <cfRule type="cellIs" dxfId="169" priority="193" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="160" priority="190" operator="equal">
+    <cfRule type="cellIs" dxfId="168" priority="194" operator="equal">
       <formula>"Normal"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="159" priority="191" operator="equal">
+    <cfRule type="cellIs" dxfId="167" priority="195" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H44">
-    <cfRule type="cellIs" dxfId="158" priority="185" operator="equal">
+    <cfRule type="cellIs" dxfId="166" priority="189" operator="equal">
       <formula>"Due/Overdue"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="157" priority="186" operator="equal">
+    <cfRule type="cellIs" dxfId="165" priority="190" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="156" priority="187" operator="equal">
+    <cfRule type="cellIs" dxfId="164" priority="191" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="155" priority="188" operator="equal">
+    <cfRule type="cellIs" dxfId="163" priority="192" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D18">
-    <cfRule type="cellIs" dxfId="154" priority="136" operator="equal">
+    <cfRule type="cellIs" dxfId="162" priority="140" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="153" priority="137" operator="equal">
+    <cfRule type="cellIs" dxfId="161" priority="141" operator="equal">
       <formula>"Normal"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="152" priority="138" operator="equal">
+    <cfRule type="cellIs" dxfId="160" priority="142" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H18">
-    <cfRule type="cellIs" dxfId="151" priority="132" operator="equal">
+    <cfRule type="cellIs" dxfId="159" priority="136" operator="equal">
       <formula>"Due/Overdue"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="150" priority="133" operator="equal">
+    <cfRule type="cellIs" dxfId="158" priority="137" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="149" priority="134" operator="equal">
+    <cfRule type="cellIs" dxfId="157" priority="138" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="148" priority="135" operator="equal">
+    <cfRule type="cellIs" dxfId="156" priority="139" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D63">
-    <cfRule type="cellIs" dxfId="147" priority="175" operator="equal">
+    <cfRule type="cellIs" dxfId="155" priority="179" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="146" priority="176" operator="equal">
+    <cfRule type="cellIs" dxfId="154" priority="180" operator="equal">
       <formula>"Normal"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="145" priority="177" operator="equal">
+    <cfRule type="cellIs" dxfId="153" priority="181" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H63">
-    <cfRule type="cellIs" dxfId="144" priority="167" operator="equal">
+    <cfRule type="cellIs" dxfId="152" priority="171" operator="equal">
       <formula>"Due/Overdue"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="143" priority="168" operator="equal">
+    <cfRule type="cellIs" dxfId="151" priority="172" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="142" priority="169" operator="equal">
+    <cfRule type="cellIs" dxfId="150" priority="173" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="141" priority="170" operator="equal">
+    <cfRule type="cellIs" dxfId="149" priority="174" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D56">
-    <cfRule type="cellIs" dxfId="140" priority="164" operator="equal">
+    <cfRule type="cellIs" dxfId="148" priority="168" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="139" priority="165" operator="equal">
+    <cfRule type="cellIs" dxfId="147" priority="169" operator="equal">
       <formula>"Normal"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="138" priority="166" operator="equal">
+    <cfRule type="cellIs" dxfId="146" priority="170" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H56">
-    <cfRule type="cellIs" dxfId="137" priority="160" operator="equal">
+    <cfRule type="cellIs" dxfId="145" priority="164" operator="equal">
       <formula>"Due/Overdue"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="136" priority="161" operator="equal">
+    <cfRule type="cellIs" dxfId="144" priority="165" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="135" priority="162" operator="equal">
+    <cfRule type="cellIs" dxfId="143" priority="166" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="134" priority="163" operator="equal">
+    <cfRule type="cellIs" dxfId="142" priority="167" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D57:D58">
-    <cfRule type="cellIs" dxfId="133" priority="157" operator="equal">
+    <cfRule type="cellIs" dxfId="141" priority="161" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="132" priority="158" operator="equal">
+    <cfRule type="cellIs" dxfId="140" priority="162" operator="equal">
       <formula>"Normal"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="131" priority="159" operator="equal">
+    <cfRule type="cellIs" dxfId="139" priority="163" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D16">
-    <cfRule type="cellIs" dxfId="130" priority="150" operator="equal">
+    <cfRule type="cellIs" dxfId="138" priority="154" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="129" priority="151" operator="equal">
+    <cfRule type="cellIs" dxfId="137" priority="155" operator="equal">
       <formula>"Normal"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="128" priority="152" operator="equal">
+    <cfRule type="cellIs" dxfId="136" priority="156" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H16">
-    <cfRule type="cellIs" dxfId="127" priority="146" operator="equal">
+    <cfRule type="cellIs" dxfId="135" priority="150" operator="equal">
       <formula>"Due/Overdue"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="126" priority="147" operator="equal">
+    <cfRule type="cellIs" dxfId="134" priority="151" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="125" priority="148" operator="equal">
+    <cfRule type="cellIs" dxfId="133" priority="152" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="124" priority="149" operator="equal">
+    <cfRule type="cellIs" dxfId="132" priority="153" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D17">
-    <cfRule type="cellIs" dxfId="123" priority="143" operator="equal">
+    <cfRule type="cellIs" dxfId="131" priority="147" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="122" priority="144" operator="equal">
+    <cfRule type="cellIs" dxfId="130" priority="148" operator="equal">
       <formula>"Normal"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="121" priority="145" operator="equal">
+    <cfRule type="cellIs" dxfId="129" priority="149" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H17">
-    <cfRule type="cellIs" dxfId="120" priority="139" operator="equal">
+    <cfRule type="cellIs" dxfId="128" priority="143" operator="equal">
       <formula>"Due/Overdue"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="119" priority="140" operator="equal">
+    <cfRule type="cellIs" dxfId="127" priority="144" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="118" priority="141" operator="equal">
+    <cfRule type="cellIs" dxfId="126" priority="145" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="117" priority="142" operator="equal">
+    <cfRule type="cellIs" dxfId="125" priority="146" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D19">
-    <cfRule type="cellIs" dxfId="116" priority="129" operator="equal">
+    <cfRule type="cellIs" dxfId="124" priority="133" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="115" priority="130" operator="equal">
+    <cfRule type="cellIs" dxfId="123" priority="134" operator="equal">
       <formula>"Normal"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="114" priority="131" operator="equal">
+    <cfRule type="cellIs" dxfId="122" priority="135" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H19">
-    <cfRule type="cellIs" dxfId="113" priority="125" operator="equal">
+    <cfRule type="cellIs" dxfId="121" priority="129" operator="equal">
       <formula>"Due/Overdue"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="112" priority="126" operator="equal">
+    <cfRule type="cellIs" dxfId="120" priority="130" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="111" priority="127" operator="equal">
+    <cfRule type="cellIs" dxfId="119" priority="131" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="110" priority="128" operator="equal">
+    <cfRule type="cellIs" dxfId="118" priority="132" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H24">
-    <cfRule type="cellIs" dxfId="109" priority="114" operator="equal">
+    <cfRule type="cellIs" dxfId="117" priority="118" operator="equal">
       <formula>"Due/Overdue"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="108" priority="115" operator="equal">
+    <cfRule type="cellIs" dxfId="116" priority="119" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="107" priority="116" operator="equal">
+    <cfRule type="cellIs" dxfId="115" priority="120" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="106" priority="117" operator="equal">
+    <cfRule type="cellIs" dxfId="114" priority="121" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D24">
-    <cfRule type="cellIs" dxfId="105" priority="111" operator="equal">
+    <cfRule type="cellIs" dxfId="113" priority="115" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="104" priority="112" operator="equal">
+    <cfRule type="cellIs" dxfId="112" priority="116" operator="equal">
       <formula>"Normal"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="103" priority="113" operator="equal">
+    <cfRule type="cellIs" dxfId="111" priority="117" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H26">
-    <cfRule type="cellIs" dxfId="102" priority="107" operator="equal">
+    <cfRule type="cellIs" dxfId="110" priority="111" operator="equal">
       <formula>"Due/Overdue"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="101" priority="108" operator="equal">
+    <cfRule type="cellIs" dxfId="109" priority="112" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="100" priority="109" operator="equal">
+    <cfRule type="cellIs" dxfId="108" priority="113" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="99" priority="110" operator="equal">
+    <cfRule type="cellIs" dxfId="107" priority="114" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H27">
-    <cfRule type="cellIs" dxfId="98" priority="103" operator="equal">
+    <cfRule type="cellIs" dxfId="106" priority="107" operator="equal">
       <formula>"Due/Overdue"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="97" priority="104" operator="equal">
+    <cfRule type="cellIs" dxfId="105" priority="108" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="96" priority="105" operator="equal">
+    <cfRule type="cellIs" dxfId="104" priority="109" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="95" priority="106" operator="equal">
+    <cfRule type="cellIs" dxfId="103" priority="110" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D32">
-    <cfRule type="cellIs" dxfId="94" priority="100" operator="equal">
+    <cfRule type="cellIs" dxfId="102" priority="104" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="93" priority="101" operator="equal">
+    <cfRule type="cellIs" dxfId="101" priority="105" operator="equal">
       <formula>"Normal"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="92" priority="102" operator="equal">
+    <cfRule type="cellIs" dxfId="100" priority="106" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H32">
-    <cfRule type="cellIs" dxfId="91" priority="96" operator="equal">
+    <cfRule type="cellIs" dxfId="99" priority="100" operator="equal">
       <formula>"Due/Overdue"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="90" priority="97" operator="equal">
+    <cfRule type="cellIs" dxfId="98" priority="101" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="89" priority="98" operator="equal">
+    <cfRule type="cellIs" dxfId="97" priority="102" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="88" priority="99" operator="equal">
+    <cfRule type="cellIs" dxfId="96" priority="103" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D33">
-    <cfRule type="cellIs" dxfId="87" priority="93" operator="equal">
+    <cfRule type="cellIs" dxfId="95" priority="97" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="86" priority="94" operator="equal">
+    <cfRule type="cellIs" dxfId="94" priority="98" operator="equal">
       <formula>"Normal"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="85" priority="95" operator="equal">
+    <cfRule type="cellIs" dxfId="93" priority="99" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H33">
-    <cfRule type="cellIs" dxfId="84" priority="89" operator="equal">
+    <cfRule type="cellIs" dxfId="92" priority="93" operator="equal">
       <formula>"Due/Overdue"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="83" priority="90" operator="equal">
+    <cfRule type="cellIs" dxfId="91" priority="94" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="82" priority="91" operator="equal">
+    <cfRule type="cellIs" dxfId="90" priority="95" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="81" priority="92" operator="equal">
+    <cfRule type="cellIs" dxfId="89" priority="96" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D34">
-    <cfRule type="cellIs" dxfId="80" priority="86" operator="equal">
+    <cfRule type="cellIs" dxfId="88" priority="90" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="79" priority="87" operator="equal">
+    <cfRule type="cellIs" dxfId="87" priority="91" operator="equal">
       <formula>"Normal"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="78" priority="88" operator="equal">
+    <cfRule type="cellIs" dxfId="86" priority="92" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H34">
-    <cfRule type="cellIs" dxfId="77" priority="82" operator="equal">
+    <cfRule type="cellIs" dxfId="85" priority="86" operator="equal">
       <formula>"Due/Overdue"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="76" priority="83" operator="equal">
+    <cfRule type="cellIs" dxfId="84" priority="87" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="75" priority="84" operator="equal">
+    <cfRule type="cellIs" dxfId="83" priority="88" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="74" priority="85" operator="equal">
+    <cfRule type="cellIs" dxfId="82" priority="89" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D39">
-    <cfRule type="cellIs" dxfId="73" priority="79" operator="equal">
+    <cfRule type="cellIs" dxfId="81" priority="83" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="72" priority="80" operator="equal">
+    <cfRule type="cellIs" dxfId="80" priority="84" operator="equal">
       <formula>"Normal"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="71" priority="81" operator="equal">
+    <cfRule type="cellIs" dxfId="79" priority="85" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H39">
-    <cfRule type="cellIs" dxfId="70" priority="75" operator="equal">
+    <cfRule type="cellIs" dxfId="78" priority="79" operator="equal">
       <formula>"Due/Overdue"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="69" priority="76" operator="equal">
+    <cfRule type="cellIs" dxfId="77" priority="80" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="68" priority="77" operator="equal">
+    <cfRule type="cellIs" dxfId="76" priority="81" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="67" priority="78" operator="equal">
+    <cfRule type="cellIs" dxfId="75" priority="82" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D45">
-    <cfRule type="cellIs" dxfId="66" priority="72" operator="equal">
+    <cfRule type="cellIs" dxfId="74" priority="76" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="65" priority="73" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="77" operator="equal">
       <formula>"Normal"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="64" priority="74" operator="equal">
+    <cfRule type="cellIs" dxfId="72" priority="78" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H45">
-    <cfRule type="cellIs" dxfId="63" priority="68" operator="equal">
+    <cfRule type="cellIs" dxfId="71" priority="72" operator="equal">
       <formula>"Due/Overdue"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="62" priority="69" operator="equal">
+    <cfRule type="cellIs" dxfId="70" priority="73" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="61" priority="70" operator="equal">
+    <cfRule type="cellIs" dxfId="69" priority="74" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="71" operator="equal">
+    <cfRule type="cellIs" dxfId="68" priority="75" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D46">
-    <cfRule type="cellIs" dxfId="59" priority="65" operator="equal">
+    <cfRule type="cellIs" dxfId="67" priority="69" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="66" operator="equal">
+    <cfRule type="cellIs" dxfId="66" priority="70" operator="equal">
       <formula>"Normal"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="57" priority="67" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="71" operator="equal">
       <formula>"Low"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D47">
+    <cfRule type="cellIs" dxfId="60" priority="62" operator="equal">
+      <formula>"High"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="59" priority="63" operator="equal">
+      <formula>"Normal"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="58" priority="64" operator="equal">
+      <formula>"Low"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H47">
+    <cfRule type="cellIs" dxfId="57" priority="58" operator="equal">
+      <formula>"Due/Overdue"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="56" priority="59" operator="equal">
+      <formula>"In Progress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="55" priority="60" operator="equal">
+      <formula>"Done"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="54" priority="61" operator="equal">
+      <formula>"Pending"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H52">
+    <cfRule type="cellIs" dxfId="53" priority="54" operator="equal">
+      <formula>"Due/Overdue"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="52" priority="55" operator="equal">
+      <formula>"In Progress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="51" priority="56" operator="equal">
+      <formula>"Done"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="50" priority="57" operator="equal">
+      <formula>"Pending"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D54">
+    <cfRule type="cellIs" dxfId="49" priority="37" operator="equal">
+      <formula>"High"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="48" priority="38" operator="equal">
+      <formula>"Normal"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="47" priority="39" operator="equal">
+      <formula>"Low"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H54">
+    <cfRule type="cellIs" dxfId="46" priority="33" operator="equal">
+      <formula>"Due/Overdue"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="45" priority="34" operator="equal">
+      <formula>"In Progress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="44" priority="35" operator="equal">
+      <formula>"Done"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="43" priority="36" operator="equal">
+      <formula>"Pending"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D53">
+    <cfRule type="cellIs" dxfId="42" priority="44" operator="equal">
+      <formula>"High"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="41" priority="45" operator="equal">
+      <formula>"Normal"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="40" priority="46" operator="equal">
+      <formula>"Low"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H53">
+    <cfRule type="cellIs" dxfId="39" priority="40" operator="equal">
+      <formula>"Due/Overdue"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="38" priority="41" operator="equal">
+      <formula>"In Progress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="37" priority="42" operator="equal">
+      <formula>"Done"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="36" priority="43" operator="equal">
+      <formula>"Pending"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D62">
+    <cfRule type="cellIs" dxfId="35" priority="9" operator="equal">
+      <formula>"High"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="34" priority="10" operator="equal">
+      <formula>"Normal"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="33" priority="11" operator="equal">
+      <formula>"Low"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H62">
+    <cfRule type="cellIs" dxfId="32" priority="5" operator="equal">
+      <formula>"Due/Overdue"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="31" priority="6" operator="equal">
+      <formula>"In Progress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="30" priority="7" operator="equal">
+      <formula>"Done"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="29" priority="8" operator="equal">
+      <formula>"Pending"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D59">
+    <cfRule type="cellIs" dxfId="28" priority="30" operator="equal">
+      <formula>"High"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="27" priority="31" operator="equal">
+      <formula>"Normal"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="26" priority="32" operator="equal">
+      <formula>"Low"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H59">
+    <cfRule type="cellIs" dxfId="25" priority="26" operator="equal">
+      <formula>"Due/Overdue"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="24" priority="27" operator="equal">
+      <formula>"In Progress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="23" priority="28" operator="equal">
+      <formula>"Done"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="22" priority="29" operator="equal">
+      <formula>"Pending"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D60">
+    <cfRule type="cellIs" dxfId="21" priority="23" operator="equal">
+      <formula>"High"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="20" priority="24" operator="equal">
+      <formula>"Normal"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="19" priority="25" operator="equal">
+      <formula>"Low"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H60">
+    <cfRule type="cellIs" dxfId="18" priority="19" operator="equal">
+      <formula>"Due/Overdue"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="17" priority="20" operator="equal">
+      <formula>"In Progress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="21" operator="equal">
+      <formula>"Done"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="15" priority="22" operator="equal">
+      <formula>"Pending"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D61">
+    <cfRule type="cellIs" dxfId="14" priority="16" operator="equal">
+      <formula>"High"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="13" priority="17" operator="equal">
+      <formula>"Normal"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="18" operator="equal">
+      <formula>"Low"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H61">
+    <cfRule type="cellIs" dxfId="11" priority="12" operator="equal">
+      <formula>"Due/Overdue"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="13" operator="equal">
+      <formula>"In Progress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="9" priority="14" operator="equal">
+      <formula>"Done"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="15" operator="equal">
+      <formula>"Pending"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H46">
-    <cfRule type="cellIs" dxfId="56" priority="61" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
       <formula>"Due/Overdue"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="55" priority="62" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="63" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="53" priority="64" operator="equal">
-      <formula>"Pending"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D47">
-    <cfRule type="cellIs" dxfId="52" priority="58" operator="equal">
-      <formula>"High"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="51" priority="59" operator="equal">
-      <formula>"Normal"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="50" priority="60" operator="equal">
-      <formula>"Low"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H47">
-    <cfRule type="cellIs" dxfId="49" priority="54" operator="equal">
-      <formula>"Due/Overdue"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="55" operator="equal">
-      <formula>"In Progress"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="47" priority="56" operator="equal">
-      <formula>"Done"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="57" operator="equal">
-      <formula>"Pending"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H52">
-    <cfRule type="cellIs" dxfId="45" priority="50" operator="equal">
-      <formula>"Due/Overdue"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="44" priority="51" operator="equal">
-      <formula>"In Progress"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="43" priority="52" operator="equal">
-      <formula>"Done"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="53" operator="equal">
-      <formula>"Pending"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D54">
-    <cfRule type="cellIs" dxfId="41" priority="33" operator="equal">
-      <formula>"High"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="34" operator="equal">
-      <formula>"Normal"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="35" operator="equal">
-      <formula>"Low"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H54">
-    <cfRule type="cellIs" dxfId="38" priority="29" operator="equal">
-      <formula>"Due/Overdue"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="30" operator="equal">
-      <formula>"In Progress"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="31" operator="equal">
-      <formula>"Done"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="35" priority="32" operator="equal">
-      <formula>"Pending"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D53">
-    <cfRule type="cellIs" dxfId="34" priority="40" operator="equal">
-      <formula>"High"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="41" operator="equal">
-      <formula>"Normal"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="42" operator="equal">
-      <formula>"Low"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H53">
-    <cfRule type="cellIs" dxfId="31" priority="36" operator="equal">
-      <formula>"Due/Overdue"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="37" operator="equal">
-      <formula>"In Progress"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="38" operator="equal">
-      <formula>"Done"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="39" operator="equal">
-      <formula>"Pending"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D62">
-    <cfRule type="cellIs" dxfId="27" priority="5" operator="equal">
-      <formula>"High"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="6" operator="equal">
-      <formula>"Normal"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="7" operator="equal">
-      <formula>"Low"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H62">
-    <cfRule type="cellIs" dxfId="24" priority="1" operator="equal">
-      <formula>"Due/Overdue"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="2" operator="equal">
-      <formula>"In Progress"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="3" operator="equal">
-      <formula>"Done"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="4" operator="equal">
-      <formula>"Pending"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D59">
-    <cfRule type="cellIs" dxfId="20" priority="26" operator="equal">
-      <formula>"High"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="27" operator="equal">
-      <formula>"Normal"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="28" operator="equal">
-      <formula>"Low"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H59">
-    <cfRule type="cellIs" dxfId="17" priority="22" operator="equal">
-      <formula>"Due/Overdue"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="23" operator="equal">
-      <formula>"In Progress"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="24" operator="equal">
-      <formula>"Done"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="25" operator="equal">
-      <formula>"Pending"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D60">
-    <cfRule type="cellIs" dxfId="13" priority="19" operator="equal">
-      <formula>"High"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="20" operator="equal">
-      <formula>"Normal"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="21" operator="equal">
-      <formula>"Low"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H60">
-    <cfRule type="cellIs" dxfId="10" priority="15" operator="equal">
-      <formula>"Due/Overdue"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="16" operator="equal">
-      <formula>"In Progress"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="17" operator="equal">
-      <formula>"Done"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="18" operator="equal">
-      <formula>"Pending"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D61">
-    <cfRule type="cellIs" dxfId="6" priority="12" operator="equal">
-      <formula>"High"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="13" operator="equal">
-      <formula>"Normal"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="14" operator="equal">
-      <formula>"Low"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H61">
-    <cfRule type="cellIs" dxfId="3" priority="8" operator="equal">
-      <formula>"Due/Overdue"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="9" operator="equal">
-      <formula>"In Progress"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="10" operator="equal">
-      <formula>"Done"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D63" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D63">
       <formula1>"Low,Normal,High"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H1:H1048576" xr:uid="{00000000-0002-0000-0100-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H1:H1048576">
       <formula1>"Pending, In Progress, Done,Due/Overdue"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="I6" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-    <hyperlink ref="I23" r:id="rId2" xr:uid="{4B9AF62C-EF0C-4C32-8334-27D2D6FEB03F}"/>
+    <hyperlink ref="I6" r:id="rId1"/>
+    <hyperlink ref="I23" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" xr3:uid="{842E5F09-E766-5B8D-85AF-A39847EA96FD}">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002559E96BE1366749B5994691468FA9F5" ma:contentTypeVersion="9" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="8e8ad5d5f5b847d36124a6739bcb066d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="bb180c85-76f3-48e0-b328-7ffec8745cdb" xmlns:ns3="9107859c-f784-45d5-9a48-227635d9abf6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="27ad90bc540ca690cb9461c6ecfab43c" ns2:_="" ns3:_="">
     <xsd:import namespace="bb180c85-76f3-48e0-b328-7ffec8745cdb"/>
@@ -11545,15 +11628,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -11563,13 +11637,38 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{42425092-60E3-46BA-9592-E936EBC78178}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7752FAE2-4C1A-4AF9-8FFF-57841E3A9384}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7752FAE2-4C1A-4AF9-8FFF-57841E3A9384}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{42425092-60E3-46BA-9592-E936EBC78178}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="bb180c85-76f3-48e0-b328-7ffec8745cdb"/>
+    <ds:schemaRef ds:uri="9107859c-f784-45d5-9a48-227635d9abf6"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7610F338-E3EB-4ACA-9F32-4582C6B5877A}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7610F338-E3EB-4ACA-9F32-4582C6B5877A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="bb180c85-76f3-48e0-b328-7ffec8745cdb"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>